<commit_message>
Have now completed manually checking TRBIV genome annotations.
</commit_message>
<xml_diff>
--- a/prokka_outputs/Manually checked annotation summary/2024-08-05_Manual Check_Nucleotide alignment Annotations.xlsx
+++ b/prokka_outputs/Manually checked annotation summary/2024-08-05_Manual Check_Nucleotide alignment Annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/prokka_outputs/Manually checked annotation summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2998" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E82B4F43-1CB8-4689-ABD5-444217A10C2E}"/>
+  <xr:revisionPtr revIDLastSave="3276" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52542966-ECCA-4A27-845E-54837AB94548}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{2726C256-0AC9-4A8B-B368-59495ADA43C2}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9538" uniqueCount="1366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9881" uniqueCount="1392">
   <si>
     <t>Type</t>
   </si>
@@ -4272,6 +4272,84 @@
   </si>
   <si>
     <t xml:space="preserve">20 matches in GenBank which were closer in length to the larger reference genome annotation. I swapped the Prokka annotation for the reference genome annotation. </t>
+  </si>
+  <si>
+    <t>10 matches in GenBank of equal length.</t>
+  </si>
+  <si>
+    <t>7 matches in Genbank for reference genome vs 4 matches in Genbank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Matches from BLASTp GenBank query. 3 were of equal size to the sequence (71 amino acids long). The others were ~80 amino acids long. Decided to keep. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 matches in GenBank. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 matches in GenBank which were larger than this sequence. &gt;100 sequences of equal/similar size matched for the referenc egenome annotation which covered the interval of this gene. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;100 matches in GenBank with genes of a equal or a similar size. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypothetical protein OR CD83 antigen as identified when isolated from other species of (susceptible?) fish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over 100 matches in Genbankof a similar size. </t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No matches in GenBank. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;100 seuqnece matches from BLASTp search compared to 8 matches for Prokka annotation which covered the same interval of this gene. Decided to use GenBank annotation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 matches in GenBank but none are of the same length. All 20bp longer. Decided not to add. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;100 sequences matched in GenBank. 10 of equal size (990 amino acids long). Others larger (&gt;1000 amino acids long). Decdied to keep. </t>
+  </si>
+  <si>
+    <t>&gt;100 matches in GenBank with genes of a equal or a similar size (445 amino acids long).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 matches in Genbank but all 12-13 amino acids longer than this gene. Decided to keep. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 matches in GenBank. Matches are equal to or closer in length to the reference genome annotation version of this gene. Copied reference genome annotation and removed Prokka version. </t>
+  </si>
+  <si>
+    <t>Hypothetial protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More matces for the larger Prokka-annotated gene compared to the reference annotated gene. Kept Prokka version. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;100 matches for reference genome annotation and Prokka annotation ranging between sequence lengths equal to both seperate annotations.Decided to keep Prokka version. </t>
+  </si>
+  <si>
+    <t>30 matches for Prokka and reference genome annotation ranging from lenghts equal to both different annotations. Decided to keep Prokka version.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 matches for gene. 2 matches for gene in refeence genome covering a similar interval on the genome. Kept Prokka annotaion and didn not add reference genome annotation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 matches for Prokka annotation but 5 for reference genome version of annotation. Updated to length of reference genome annotation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 matches in GenBank for Prokka annotation and 5 and zero matches for two genes in reference genome covering this interval. Kept Prokka annotation and did not add reference genome annotations. </t>
+  </si>
+  <si>
+    <t>2 matches in Genbank of equal length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;100 matches in GenBank for Prokka and reference genome version of thie gene. The matches were more similar in length to the reference genome version so I swapped the Prokka version for the refernce genome version. </t>
+  </si>
+  <si>
+    <t>More matches in GenBank for the Prokka version f this gene (as opposed to the reference genome annotation)</t>
   </si>
 </sst>
 </file>
@@ -4828,7 +4906,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4933,7 +5011,14 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -48062,8 +48147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3FEEE8-70D8-4BA8-8B68-9FBAA402446E}">
   <dimension ref="A1:P236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="C233" sqref="A233:XFD234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51220,7 +51305,7 @@
       <c r="G82" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="H82" s="44">
+      <c r="H82" s="7">
         <v>41361</v>
       </c>
       <c r="I82" s="11">
@@ -51778,37 +51863,49 @@
       <c r="O97" s="7"/>
       <c r="P97" s="7"/>
     </row>
-    <row r="98" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C98" s="8">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" s="7">
         <v>46939</v>
       </c>
-      <c r="D98" s="8">
+      <c r="D98" s="7">
         <v>47109</v>
       </c>
-      <c r="E98" s="8">
+      <c r="E98" s="7">
         <v>171</v>
       </c>
-      <c r="F98" s="8"/>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
-      <c r="I98" s="8"/>
-      <c r="J98" s="8"/>
-      <c r="K98" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L98" s="8" t="s">
+      <c r="F98" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G98" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H98" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I98" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J98" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K98" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L98" s="7" t="s">
         <v>1226</v>
       </c>
-      <c r="M98" s="9"/>
-      <c r="N98" s="8"/>
-      <c r="O98" s="8"/>
-      <c r="P98" s="8"/>
+      <c r="M98" s="2" t="s">
+        <v>1366</v>
+      </c>
+      <c r="N98" s="7"/>
+      <c r="O98" s="7"/>
+      <c r="P98" s="7"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
@@ -51928,11 +52025,21 @@
       <c r="E102" s="7">
         <v>501</v>
       </c>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7"/>
-      <c r="H102" s="7"/>
-      <c r="I102" s="7"/>
-      <c r="J102" s="7"/>
+      <c r="F102" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G102" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H102" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I102" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J102" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K102" s="7" t="s">
         <v>7</v>
       </c>
@@ -51974,7 +52081,7 @@
       <c r="O103" s="7"/>
       <c r="P103" s="7"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
         <v>347</v>
       </c>
@@ -51990,18 +52097,30 @@
       <c r="E104" s="7">
         <v>192</v>
       </c>
-      <c r="F104" s="7"/>
-      <c r="G104" s="7"/>
-      <c r="H104" s="7"/>
-      <c r="I104" s="7"/>
-      <c r="J104" s="7"/>
+      <c r="F104" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G104" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H104" s="11">
+        <v>48327</v>
+      </c>
+      <c r="I104" s="11">
+        <v>48542</v>
+      </c>
+      <c r="J104" s="11">
+        <v>216</v>
+      </c>
       <c r="K104" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L104" s="7" t="s">
         <v>1232</v>
       </c>
-      <c r="M104" s="2"/>
+      <c r="M104" s="2" t="s">
+        <v>1367</v>
+      </c>
       <c r="N104" s="7"/>
       <c r="O104" s="7"/>
       <c r="P104" s="7"/>
@@ -52052,11 +52171,21 @@
       <c r="E106" s="7">
         <v>927</v>
       </c>
-      <c r="F106" s="7"/>
-      <c r="G106" s="7"/>
-      <c r="H106" s="7"/>
-      <c r="I106" s="7"/>
-      <c r="J106" s="7"/>
+      <c r="F106" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G106" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H106" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I106" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J106" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K106" s="7" t="s">
         <v>7</v>
       </c>
@@ -52114,11 +52243,21 @@
       <c r="E108" s="7">
         <v>924</v>
       </c>
-      <c r="F108" s="7"/>
-      <c r="G108" s="7"/>
-      <c r="H108" s="7"/>
-      <c r="I108" s="7"/>
-      <c r="J108" s="7"/>
+      <c r="F108" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G108" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H108" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I108" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J108" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K108" s="7" t="s">
         <v>7</v>
       </c>
@@ -52176,11 +52315,21 @@
       <c r="E110" s="7">
         <v>648</v>
       </c>
-      <c r="F110" s="7"/>
-      <c r="G110" s="7"/>
-      <c r="H110" s="7"/>
-      <c r="I110" s="7"/>
-      <c r="J110" s="7"/>
+      <c r="F110" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G110" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H110" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I110" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J110" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K110" s="7" t="s">
         <v>7</v>
       </c>
@@ -52238,11 +52387,21 @@
       <c r="E112" s="7">
         <v>261</v>
       </c>
-      <c r="F112" s="7"/>
-      <c r="G112" s="7"/>
-      <c r="H112" s="7"/>
-      <c r="I112" s="7"/>
-      <c r="J112" s="7"/>
+      <c r="F112" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G112" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H112" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I112" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J112" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K112" s="7" t="s">
         <v>7</v>
       </c>
@@ -52254,37 +52413,49 @@
       <c r="O112" s="7"/>
       <c r="P112" s="7"/>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A113" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B113" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C113" s="7">
+    <row r="113" spans="1:16" s="46" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B113" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C113" s="44">
         <v>51331</v>
       </c>
-      <c r="D113" s="7">
+      <c r="D113" s="44">
         <v>51537</v>
       </c>
-      <c r="E113" s="7">
+      <c r="E113" s="44">
         <v>207</v>
       </c>
-      <c r="F113" s="7"/>
-      <c r="G113" s="7"/>
-      <c r="H113" s="7"/>
-      <c r="I113" s="7"/>
-      <c r="J113" s="7"/>
-      <c r="K113" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L113" s="7" t="s">
+      <c r="F113" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G113" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="H113" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I113" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J113" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K113" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L113" s="44" t="s">
         <v>1241</v>
       </c>
-      <c r="M113" s="2"/>
-      <c r="N113" s="7"/>
-      <c r="O113" s="7"/>
-      <c r="P113" s="7"/>
+      <c r="M113" s="45" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N113" s="44"/>
+      <c r="O113" s="44"/>
+      <c r="P113" s="44"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
@@ -52332,11 +52503,21 @@
       <c r="E115" s="7">
         <v>516</v>
       </c>
-      <c r="F115" s="7"/>
-      <c r="G115" s="7"/>
-      <c r="H115" s="7"/>
-      <c r="I115" s="7"/>
-      <c r="J115" s="7"/>
+      <c r="F115" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I115" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J115" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K115" s="7" t="s">
         <v>7</v>
       </c>
@@ -52394,11 +52575,22 @@
       <c r="E117" s="7">
         <v>804</v>
       </c>
-      <c r="F117" s="7"/>
-      <c r="G117" s="7"/>
-      <c r="H117" s="7"/>
-      <c r="I117" s="7"/>
-      <c r="J117" s="7"/>
+      <c r="F117" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G117" s="7" t="str">
+        <f>B116</f>
+        <v>putative replication factor CDS</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I117" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J117" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K117" s="7" t="s">
         <v>7</v>
       </c>
@@ -52456,11 +52648,21 @@
       <c r="E119" s="7">
         <v>3450</v>
       </c>
-      <c r="F119" s="7"/>
-      <c r="G119" s="7"/>
-      <c r="H119" s="7"/>
-      <c r="I119" s="7"/>
-      <c r="J119" s="7"/>
+      <c r="F119" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I119" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J119" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K119" s="7" t="s">
         <v>7</v>
       </c>
@@ -52488,18 +52690,30 @@
       <c r="E120" s="7">
         <v>369</v>
       </c>
-      <c r="F120" s="7"/>
-      <c r="G120" s="7"/>
-      <c r="H120" s="7"/>
-      <c r="I120" s="7"/>
-      <c r="J120" s="7"/>
+      <c r="F120" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G120" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H120" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I120" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J120" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K120" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L120" s="7" t="s">
         <v>1248</v>
       </c>
-      <c r="M120" s="2"/>
+      <c r="M120" s="2" t="s">
+        <v>1369</v>
+      </c>
       <c r="N120" s="7"/>
       <c r="O120" s="7"/>
       <c r="P120" s="7"/>
@@ -52550,11 +52764,22 @@
       <c r="E122" s="7">
         <v>2649</v>
       </c>
-      <c r="F122" s="7"/>
-      <c r="G122" s="7"/>
-      <c r="H122" s="7"/>
-      <c r="I122" s="7"/>
-      <c r="J122" s="7"/>
+      <c r="F122" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G122" s="7" t="str">
+        <f>B121</f>
+        <v>SNF2 family helicase CDS</v>
+      </c>
+      <c r="H122" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I122" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J122" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K122" s="7" t="s">
         <v>7</v>
       </c>
@@ -52596,7 +52821,7 @@
       <c r="O123" s="7"/>
       <c r="P123" s="7"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
         <v>347</v>
       </c>
@@ -52612,11 +52837,22 @@
       <c r="E124" s="7">
         <v>1473</v>
       </c>
-      <c r="F124" s="7"/>
-      <c r="G124" s="7"/>
-      <c r="H124" s="7"/>
-      <c r="I124" s="7"/>
-      <c r="J124" s="7"/>
+      <c r="F124" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G124" s="7" t="str">
+        <f>B123</f>
+        <v>mRNA capping enzyme CDS</v>
+      </c>
+      <c r="H124" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I124" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J124" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K124" s="7" t="s">
         <v>7</v>
       </c>
@@ -52628,7 +52864,7 @@
       <c r="O124" s="7"/>
       <c r="P124" s="7"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="7" t="s">
         <v>347</v>
       </c>
@@ -52644,23 +52880,35 @@
       <c r="E125" s="7">
         <v>264</v>
       </c>
-      <c r="F125" s="7"/>
-      <c r="G125" s="7"/>
-      <c r="H125" s="7"/>
-      <c r="I125" s="7"/>
-      <c r="J125" s="7"/>
+      <c r="F125" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G125" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="H125" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I125" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J125" s="11" t="s">
+        <v>213</v>
+      </c>
       <c r="K125" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L125" s="7" t="s">
         <v>1251</v>
       </c>
-      <c r="M125" s="2"/>
+      <c r="M125" s="2" t="s">
+        <v>1370</v>
+      </c>
       <c r="N125" s="7"/>
       <c r="O125" s="7"/>
       <c r="P125" s="7"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
         <v>348</v>
       </c>
@@ -52676,16 +52924,28 @@
       <c r="E126" s="7">
         <v>480</v>
       </c>
-      <c r="F126" s="7"/>
-      <c r="G126" s="7"/>
-      <c r="H126" s="7"/>
-      <c r="I126" s="7"/>
-      <c r="J126" s="7"/>
+      <c r="F126" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G126" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="H126" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="I126" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J126" s="15" t="s">
+        <v>169</v>
+      </c>
       <c r="K126" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L126" s="7"/>
-      <c r="M126" s="2"/>
+      <c r="M126" s="2" t="s">
+        <v>1371</v>
+      </c>
       <c r="N126" s="7"/>
       <c r="O126" s="7"/>
       <c r="P126" s="7"/>
@@ -52736,11 +52996,22 @@
       <c r="E128" s="7">
         <v>1041</v>
       </c>
-      <c r="F128" s="7"/>
-      <c r="G128" s="7"/>
-      <c r="H128" s="7"/>
-      <c r="I128" s="7"/>
-      <c r="J128" s="7"/>
+      <c r="F128" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G128" s="7" t="str">
+        <f>B127</f>
+        <v>RING-finger-containing E3 ubiquitin ligase CDS</v>
+      </c>
+      <c r="H128" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I128" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J128" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K128" s="7" t="s">
         <v>7</v>
       </c>
@@ -52782,7 +53053,7 @@
       <c r="O129" s="7"/>
       <c r="P129" s="7"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
         <v>347</v>
       </c>
@@ -52798,18 +53069,30 @@
       <c r="E130" s="7">
         <v>567</v>
       </c>
-      <c r="F130" s="7"/>
-      <c r="G130" s="7"/>
-      <c r="H130" s="7"/>
-      <c r="I130" s="7"/>
-      <c r="J130" s="7"/>
+      <c r="F130" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>1372</v>
+      </c>
+      <c r="H130" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I130" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J130" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K130" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L130" s="7" t="s">
         <v>1254</v>
       </c>
-      <c r="M130" s="2"/>
+      <c r="M130" s="2" t="s">
+        <v>1373</v>
+      </c>
       <c r="N130" s="7"/>
       <c r="O130" s="7"/>
       <c r="P130" s="7"/>
@@ -52860,11 +53143,21 @@
       <c r="E132" s="7">
         <v>1443</v>
       </c>
-      <c r="F132" s="7"/>
-      <c r="G132" s="7"/>
-      <c r="H132" s="7"/>
-      <c r="I132" s="7"/>
-      <c r="J132" s="7"/>
+      <c r="F132" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G132" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H132" s="7" t="s">
+        <v>1374</v>
+      </c>
+      <c r="I132" s="7" t="s">
+        <v>1374</v>
+      </c>
+      <c r="J132" s="7" t="s">
+        <v>1374</v>
+      </c>
       <c r="K132" s="7" t="s">
         <v>7</v>
       </c>
@@ -52922,18 +53215,30 @@
       <c r="E134" s="7">
         <v>294</v>
       </c>
-      <c r="F134" s="7"/>
-      <c r="G134" s="7"/>
-      <c r="H134" s="7"/>
-      <c r="I134" s="7"/>
-      <c r="J134" s="7"/>
+      <c r="F134" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G134" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="H134" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I134" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="J134" s="11" t="s">
+        <v>213</v>
+      </c>
       <c r="K134" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L134" s="7" t="s">
         <v>1258</v>
       </c>
-      <c r="M134" s="2"/>
+      <c r="M134" s="2" t="s">
+        <v>1375</v>
+      </c>
       <c r="N134" s="7"/>
       <c r="O134" s="7"/>
       <c r="P134" s="7"/>
@@ -52984,11 +53289,21 @@
       <c r="E136" s="7">
         <v>1611</v>
       </c>
-      <c r="F136" s="7"/>
-      <c r="G136" s="7"/>
-      <c r="H136" s="7"/>
-      <c r="I136" s="7"/>
-      <c r="J136" s="7"/>
+      <c r="F136" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G136" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H136" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I136" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J136" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K136" s="7" t="s">
         <v>7</v>
       </c>
@@ -53030,7 +53345,7 @@
       <c r="O137" s="7"/>
       <c r="P137" s="7"/>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
         <v>347</v>
       </c>
@@ -53046,18 +53361,30 @@
       <c r="E138" s="7">
         <v>420</v>
       </c>
-      <c r="F138" s="7"/>
-      <c r="G138" s="7"/>
-      <c r="H138" s="7"/>
-      <c r="I138" s="7"/>
-      <c r="J138" s="7"/>
+      <c r="F138" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G138" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H138" s="11">
+        <v>67509</v>
+      </c>
+      <c r="I138" s="7">
+        <v>67940</v>
+      </c>
+      <c r="J138" s="11">
+        <v>432</v>
+      </c>
       <c r="K138" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L138" s="7" t="s">
         <v>1262</v>
       </c>
-      <c r="M138" s="2"/>
+      <c r="M138" s="2" t="s">
+        <v>1376</v>
+      </c>
       <c r="N138" s="7"/>
       <c r="O138" s="7"/>
       <c r="P138" s="7"/>
@@ -53108,11 +53435,21 @@
       <c r="E140" s="7">
         <v>1023</v>
       </c>
-      <c r="F140" s="7"/>
-      <c r="G140" s="7"/>
-      <c r="H140" s="7"/>
-      <c r="I140" s="7"/>
-      <c r="J140" s="7"/>
+      <c r="F140" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G140" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H140" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I140" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J140" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K140" s="7" t="s">
         <v>9</v>
       </c>
@@ -53124,7 +53461,7 @@
       <c r="O140" s="7"/>
       <c r="P140" s="7"/>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>348</v>
       </c>
@@ -53149,12 +53486,14 @@
         <v>7</v>
       </c>
       <c r="L141" s="7"/>
-      <c r="M141" s="2"/>
+      <c r="M141" s="2" t="s">
+        <v>1377</v>
+      </c>
       <c r="N141" s="7"/>
       <c r="O141" s="7"/>
       <c r="P141" s="7"/>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>347</v>
       </c>
@@ -53170,18 +53509,30 @@
       <c r="E142" s="7">
         <v>2973</v>
       </c>
-      <c r="F142" s="7"/>
-      <c r="G142" s="7"/>
-      <c r="H142" s="7"/>
-      <c r="I142" s="7"/>
-      <c r="J142" s="7"/>
+      <c r="F142" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G142" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H142" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I142" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J142" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K142" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L142" s="7" t="s">
         <v>1266</v>
       </c>
-      <c r="M142" s="2"/>
+      <c r="M142" s="2" t="s">
+        <v>1378</v>
+      </c>
       <c r="N142" s="7"/>
       <c r="O142" s="7"/>
       <c r="P142" s="7"/>
@@ -53246,7 +53597,7 @@
       <c r="O144" s="7"/>
       <c r="P144" s="7"/>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A145" s="7" t="s">
         <v>347</v>
       </c>
@@ -53262,18 +53613,31 @@
       <c r="E145" s="7">
         <v>1335</v>
       </c>
-      <c r="F145" s="7"/>
-      <c r="G145" s="7"/>
-      <c r="H145" s="7"/>
-      <c r="I145" s="7"/>
-      <c r="J145" s="7"/>
+      <c r="F145" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G145" s="7" t="str">
+        <f>B144</f>
+        <v>ankyrin repeat-containing protein CDS</v>
+      </c>
+      <c r="H145" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I145" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J145" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K145" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L145" s="7" t="s">
         <v>1268</v>
       </c>
-      <c r="M145" s="2"/>
+      <c r="M145" s="2" t="s">
+        <v>1379</v>
+      </c>
       <c r="N145" s="7"/>
       <c r="O145" s="7"/>
       <c r="P145" s="7"/>
@@ -53308,7 +53672,7 @@
       <c r="O146" s="7"/>
       <c r="P146" s="7"/>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
         <v>347</v>
       </c>
@@ -53324,11 +53688,21 @@
       <c r="E147" s="7">
         <v>465</v>
       </c>
-      <c r="F147" s="7"/>
-      <c r="G147" s="7"/>
-      <c r="H147" s="7"/>
-      <c r="I147" s="7"/>
-      <c r="J147" s="7"/>
+      <c r="F147" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G147" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H147" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I147" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J147" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K147" s="7" t="s">
         <v>9</v>
       </c>
@@ -53340,7 +53714,7 @@
       <c r="O147" s="7"/>
       <c r="P147" s="7"/>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A148" s="7" t="s">
         <v>347</v>
       </c>
@@ -53356,18 +53730,30 @@
       <c r="E148" s="7">
         <v>177</v>
       </c>
-      <c r="F148" s="7"/>
-      <c r="G148" s="7"/>
-      <c r="H148" s="7"/>
-      <c r="I148" s="7"/>
-      <c r="J148" s="7"/>
+      <c r="F148" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G148" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H148" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I148" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J148" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K148" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L148" s="7" t="s">
         <v>1271</v>
       </c>
-      <c r="M148" s="2"/>
+      <c r="M148" s="2" t="s">
+        <v>1380</v>
+      </c>
       <c r="N148" s="7"/>
       <c r="O148" s="7"/>
       <c r="P148" s="7"/>
@@ -53448,11 +53834,21 @@
       <c r="E151" s="7">
         <v>354</v>
       </c>
-      <c r="F151" s="7"/>
-      <c r="G151" s="7"/>
-      <c r="H151" s="7"/>
-      <c r="I151" s="7"/>
-      <c r="J151" s="7"/>
+      <c r="F151" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G151" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H151" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I151" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J151" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K151" s="7" t="s">
         <v>9</v>
       </c>
@@ -53510,11 +53906,21 @@
       <c r="E153" s="7">
         <v>498</v>
       </c>
-      <c r="F153" s="7"/>
-      <c r="G153" s="7"/>
-      <c r="H153" s="7"/>
-      <c r="I153" s="7"/>
-      <c r="J153" s="7"/>
+      <c r="F153" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G153" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H153" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I153" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J153" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K153" s="7" t="s">
         <v>9</v>
       </c>
@@ -53572,11 +53978,21 @@
       <c r="E155" s="7">
         <v>1107</v>
       </c>
-      <c r="F155" s="7"/>
-      <c r="G155" s="7"/>
-      <c r="H155" s="7"/>
-      <c r="I155" s="7"/>
-      <c r="J155" s="7"/>
+      <c r="F155" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G155" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H155" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I155" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J155" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K155" s="7" t="s">
         <v>7</v>
       </c>
@@ -53634,11 +54050,21 @@
       <c r="E157" s="7">
         <v>360</v>
       </c>
-      <c r="F157" s="7"/>
-      <c r="G157" s="7"/>
-      <c r="H157" s="7"/>
-      <c r="I157" s="7"/>
-      <c r="J157" s="7"/>
+      <c r="F157" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G157" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H157" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I157" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J157" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K157" s="7" t="s">
         <v>9</v>
       </c>
@@ -53696,11 +54122,21 @@
       <c r="E159" s="7">
         <v>1356</v>
       </c>
-      <c r="F159" s="7"/>
-      <c r="G159" s="7"/>
-      <c r="H159" s="7"/>
-      <c r="I159" s="7"/>
-      <c r="J159" s="7"/>
+      <c r="F159" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G159" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H159" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I159" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J159" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K159" s="7" t="s">
         <v>7</v>
       </c>
@@ -53742,7 +54178,7 @@
       <c r="O160" s="7"/>
       <c r="P160" s="7"/>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A161" s="7" t="s">
         <v>347</v>
       </c>
@@ -53758,207 +54194,251 @@
       <c r="E161" s="7">
         <v>393</v>
       </c>
-      <c r="F161" s="7"/>
-      <c r="G161" s="7"/>
-      <c r="H161" s="7"/>
-      <c r="I161" s="7"/>
-      <c r="J161" s="7"/>
+      <c r="F161" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G161" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="H161" s="11">
+        <v>78324</v>
+      </c>
+      <c r="I161" s="7">
+        <v>78842</v>
+      </c>
+      <c r="J161" s="11">
+        <v>519</v>
+      </c>
       <c r="K161" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L161" s="7" t="s">
         <v>1284</v>
       </c>
-      <c r="M161" s="2"/>
+      <c r="M161" s="2" t="s">
+        <v>1381</v>
+      </c>
       <c r="N161" s="7"/>
       <c r="O161" s="7"/>
       <c r="P161" s="7"/>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A162" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B162" s="7" t="s">
+    <row r="162" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B162" s="44" t="s">
         <v>1285</v>
       </c>
-      <c r="C162" s="7">
+      <c r="C162" s="44">
         <v>78839</v>
       </c>
-      <c r="D162" s="7">
+      <c r="D162" s="44">
         <v>79303</v>
       </c>
-      <c r="E162" s="7">
+      <c r="E162" s="44">
         <v>465</v>
       </c>
-      <c r="F162" s="7"/>
-      <c r="G162" s="7"/>
-      <c r="H162" s="7"/>
-      <c r="I162" s="7"/>
-      <c r="J162" s="7"/>
-      <c r="K162" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L162" s="7"/>
-      <c r="M162" s="2"/>
-      <c r="N162" s="7"/>
-      <c r="O162" s="7"/>
-      <c r="P162" s="7"/>
-    </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A163" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B163" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C163" s="7">
+      <c r="F162" s="44"/>
+      <c r="G162" s="44"/>
+      <c r="H162" s="44"/>
+      <c r="I162" s="44"/>
+      <c r="J162" s="44"/>
+      <c r="K162" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L162" s="44"/>
+      <c r="M162" s="45"/>
+      <c r="N162" s="44"/>
+      <c r="O162" s="44"/>
+      <c r="P162" s="44"/>
+    </row>
+    <row r="163" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B163" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C163" s="44">
         <v>78839</v>
       </c>
-      <c r="D163" s="7">
+      <c r="D163" s="44">
         <v>79303</v>
       </c>
-      <c r="E163" s="7">
+      <c r="E163" s="44">
         <v>465</v>
       </c>
-      <c r="F163" s="7"/>
-      <c r="G163" s="7"/>
-      <c r="H163" s="7"/>
-      <c r="I163" s="7"/>
-      <c r="J163" s="7"/>
-      <c r="K163" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L163" s="7" t="s">
+      <c r="F163" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="G163" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="H163" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I163" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J163" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K163" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L163" s="44" t="s">
         <v>1286</v>
       </c>
-      <c r="M163" s="2"/>
-      <c r="N163" s="7"/>
-      <c r="O163" s="7"/>
-      <c r="P163" s="7"/>
-    </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A164" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B164" s="7" t="s">
+      <c r="M163" s="45"/>
+      <c r="N163" s="44"/>
+      <c r="O163" s="44"/>
+      <c r="P163" s="44"/>
+    </row>
+    <row r="164" spans="1:16" s="46" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B164" s="44" t="s">
         <v>1287</v>
       </c>
-      <c r="C164" s="7">
+      <c r="C164" s="44">
         <v>79263</v>
       </c>
-      <c r="D164" s="7">
+      <c r="D164" s="44">
         <v>80066</v>
       </c>
-      <c r="E164" s="7">
+      <c r="E164" s="44">
         <v>804</v>
       </c>
-      <c r="F164" s="7"/>
-      <c r="G164" s="7"/>
-      <c r="H164" s="7"/>
-      <c r="I164" s="7"/>
-      <c r="J164" s="7"/>
-      <c r="K164" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L164" s="7"/>
-      <c r="M164" s="2"/>
-      <c r="N164" s="7"/>
-      <c r="O164" s="7"/>
-      <c r="P164" s="7"/>
-    </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A165" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B165" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C165" s="7">
+      <c r="F164" s="44"/>
+      <c r="G164" s="44"/>
+      <c r="H164" s="44"/>
+      <c r="I164" s="44"/>
+      <c r="J164" s="44"/>
+      <c r="K164" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L164" s="44"/>
+      <c r="M164" s="45"/>
+      <c r="N164" s="44"/>
+      <c r="O164" s="44"/>
+      <c r="P164" s="44"/>
+    </row>
+    <row r="165" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B165" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C165" s="44">
         <v>79296</v>
       </c>
-      <c r="D165" s="7">
+      <c r="D165" s="44">
         <v>80066</v>
       </c>
-      <c r="E165" s="7">
+      <c r="E165" s="44">
         <v>771</v>
       </c>
-      <c r="F165" s="7"/>
-      <c r="G165" s="7"/>
-      <c r="H165" s="7"/>
-      <c r="I165" s="7"/>
-      <c r="J165" s="7"/>
-      <c r="K165" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L165" s="7" t="s">
+      <c r="F165" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G165" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="H165" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I165" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J165" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K165" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L165" s="44" t="s">
         <v>1288</v>
       </c>
-      <c r="M165" s="2"/>
-      <c r="N165" s="7"/>
-      <c r="O165" s="7"/>
-      <c r="P165" s="7"/>
-    </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A166" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B166" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C166" s="7">
+      <c r="M165" s="45"/>
+      <c r="N165" s="44"/>
+      <c r="O165" s="44"/>
+      <c r="P165" s="44"/>
+    </row>
+    <row r="166" spans="1:16" s="46" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A166" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B166" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C166" s="44">
         <v>80063</v>
       </c>
-      <c r="D166" s="7">
+      <c r="D166" s="44">
         <v>80476</v>
       </c>
-      <c r="E166" s="7">
+      <c r="E166" s="44">
         <v>414</v>
       </c>
-      <c r="F166" s="7"/>
-      <c r="G166" s="7"/>
-      <c r="H166" s="7"/>
-      <c r="I166" s="7"/>
-      <c r="J166" s="7"/>
-      <c r="K166" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L166" s="7" t="s">
+      <c r="F166" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G166" s="44" t="s">
+        <v>1382</v>
+      </c>
+      <c r="H166" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I166" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J166" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K166" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L166" s="44" t="s">
         <v>1289</v>
       </c>
-      <c r="M166" s="2"/>
-      <c r="N166" s="7"/>
-      <c r="O166" s="7"/>
-      <c r="P166" s="7"/>
-    </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A167" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B167" s="7" t="s">
+      <c r="M166" s="45" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N166" s="44"/>
+      <c r="O166" s="44"/>
+      <c r="P166" s="44"/>
+    </row>
+    <row r="167" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B167" s="44" t="s">
         <v>1290</v>
       </c>
-      <c r="C167" s="7">
+      <c r="C167" s="44">
         <v>80256</v>
       </c>
-      <c r="D167" s="7">
+      <c r="D167" s="44">
         <v>80573</v>
       </c>
-      <c r="E167" s="7">
+      <c r="E167" s="44">
         <v>318</v>
       </c>
-      <c r="F167" s="7"/>
-      <c r="G167" s="7"/>
-      <c r="H167" s="7"/>
-      <c r="I167" s="7"/>
-      <c r="J167" s="7"/>
-      <c r="K167" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L167" s="7"/>
-      <c r="M167" s="2"/>
-      <c r="N167" s="7"/>
-      <c r="O167" s="7"/>
-      <c r="P167" s="7"/>
+      <c r="F167" s="44"/>
+      <c r="G167" s="44"/>
+      <c r="H167" s="44"/>
+      <c r="I167" s="44"/>
+      <c r="J167" s="44"/>
+      <c r="K167" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L167" s="44"/>
+      <c r="M167" s="45"/>
+      <c r="N167" s="44"/>
+      <c r="O167" s="44"/>
+      <c r="P167" s="44"/>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168" s="7" t="s">
@@ -54006,11 +54486,21 @@
       <c r="E169" s="7">
         <v>1569</v>
       </c>
-      <c r="F169" s="7"/>
-      <c r="G169" s="7"/>
-      <c r="H169" s="7"/>
-      <c r="I169" s="7"/>
-      <c r="J169" s="7"/>
+      <c r="F169" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G169" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H169" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I169" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J169" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K169" s="7" t="s">
         <v>9</v>
       </c>
@@ -54068,11 +54558,21 @@
       <c r="E171" s="7">
         <v>1017</v>
       </c>
-      <c r="F171" s="7"/>
-      <c r="G171" s="7"/>
-      <c r="H171" s="7"/>
-      <c r="I171" s="7"/>
-      <c r="J171" s="7"/>
+      <c r="F171" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G171" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H171" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I171" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J171" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K171" s="7" t="s">
         <v>7</v>
       </c>
@@ -54084,67 +54584,77 @@
       <c r="O171" s="7"/>
       <c r="P171" s="7"/>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A172" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B172" s="7" t="s">
+    <row r="172" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B172" s="44" t="s">
         <v>1295</v>
       </c>
-      <c r="C172" s="7">
+      <c r="C172" s="44">
         <v>83094</v>
       </c>
-      <c r="D172" s="7">
+      <c r="D172" s="44">
         <v>83273</v>
       </c>
-      <c r="E172" s="7">
+      <c r="E172" s="44">
         <v>180</v>
       </c>
-      <c r="F172" s="7"/>
-      <c r="G172" s="7"/>
-      <c r="H172" s="7"/>
-      <c r="I172" s="7"/>
-      <c r="J172" s="7"/>
-      <c r="K172" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L172" s="7"/>
-      <c r="M172" s="2"/>
-      <c r="N172" s="7"/>
-      <c r="O172" s="7"/>
-      <c r="P172" s="7"/>
-    </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A173" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B173" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C173" s="7">
+      <c r="F172" s="44"/>
+      <c r="G172" s="44"/>
+      <c r="H172" s="44"/>
+      <c r="I172" s="44"/>
+      <c r="J172" s="44"/>
+      <c r="K172" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L172" s="44"/>
+      <c r="M172" s="45"/>
+      <c r="N172" s="44"/>
+      <c r="O172" s="44"/>
+      <c r="P172" s="44"/>
+    </row>
+    <row r="173" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B173" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" s="44">
         <v>83103</v>
       </c>
-      <c r="D173" s="7">
+      <c r="D173" s="44">
         <v>83273</v>
       </c>
-      <c r="E173" s="7">
+      <c r="E173" s="44">
         <v>171</v>
       </c>
-      <c r="F173" s="7"/>
-      <c r="G173" s="7"/>
-      <c r="H173" s="7"/>
-      <c r="I173" s="7"/>
-      <c r="J173" s="7"/>
-      <c r="K173" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L173" s="7" t="s">
+      <c r="F173" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G173" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H173" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I173" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J173" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K173" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L173" s="44" t="s">
         <v>1296</v>
       </c>
-      <c r="M173" s="2"/>
-      <c r="N173" s="7"/>
-      <c r="O173" s="7"/>
-      <c r="P173" s="7"/>
+      <c r="M173" s="45"/>
+      <c r="N173" s="44"/>
+      <c r="O173" s="44"/>
+      <c r="P173" s="44"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
@@ -54192,11 +54702,21 @@
       <c r="E175" s="7">
         <v>927</v>
       </c>
-      <c r="F175" s="7"/>
-      <c r="G175" s="7"/>
-      <c r="H175" s="7"/>
-      <c r="I175" s="7"/>
-      <c r="J175" s="7"/>
+      <c r="F175" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G175" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H175" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I175" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J175" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K175" s="7" t="s">
         <v>7</v>
       </c>
@@ -54254,11 +54774,21 @@
       <c r="E177" s="7">
         <v>498</v>
       </c>
-      <c r="F177" s="7"/>
-      <c r="G177" s="7"/>
-      <c r="H177" s="7"/>
-      <c r="I177" s="7"/>
-      <c r="J177" s="7"/>
+      <c r="F177" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G177" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H177" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I177" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J177" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K177" s="7" t="s">
         <v>7</v>
       </c>
@@ -54316,11 +54846,21 @@
       <c r="E179" s="7">
         <v>1170</v>
       </c>
-      <c r="F179" s="7"/>
-      <c r="G179" s="7"/>
-      <c r="H179" s="7"/>
-      <c r="I179" s="7"/>
-      <c r="J179" s="7"/>
+      <c r="F179" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G179" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H179" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I179" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J179" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K179" s="7" t="s">
         <v>7</v>
       </c>
@@ -54332,67 +54872,67 @@
       <c r="O179" s="7"/>
       <c r="P179" s="7"/>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A180" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B180" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C180" s="7">
+    <row r="180" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180" s="8">
         <v>85901</v>
       </c>
-      <c r="D180" s="7">
+      <c r="D180" s="8">
         <v>86638</v>
       </c>
-      <c r="E180" s="7">
+      <c r="E180" s="8">
         <v>738</v>
       </c>
-      <c r="F180" s="7"/>
-      <c r="G180" s="7"/>
-      <c r="H180" s="7"/>
-      <c r="I180" s="7"/>
-      <c r="J180" s="7"/>
-      <c r="K180" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L180" s="7" t="s">
+      <c r="F180" s="8"/>
+      <c r="G180" s="8"/>
+      <c r="H180" s="8"/>
+      <c r="I180" s="8"/>
+      <c r="J180" s="8"/>
+      <c r="K180" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L180" s="8" t="s">
         <v>1303</v>
       </c>
-      <c r="M180" s="2"/>
-      <c r="N180" s="7"/>
-      <c r="O180" s="7"/>
-      <c r="P180" s="7"/>
-    </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A181" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B181" s="7" t="s">
+      <c r="M180" s="9"/>
+      <c r="N180" s="8"/>
+      <c r="O180" s="8"/>
+      <c r="P180" s="8"/>
+    </row>
+    <row r="181" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B181" s="8" t="s">
         <v>1304</v>
       </c>
-      <c r="C181" s="7">
+      <c r="C181" s="8">
         <v>85901</v>
       </c>
-      <c r="D181" s="7">
+      <c r="D181" s="8">
         <v>86653</v>
       </c>
-      <c r="E181" s="7">
+      <c r="E181" s="8">
         <v>753</v>
       </c>
-      <c r="F181" s="7"/>
-      <c r="G181" s="7"/>
-      <c r="H181" s="7"/>
-      <c r="I181" s="7"/>
-      <c r="J181" s="7"/>
-      <c r="K181" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L181" s="7"/>
-      <c r="M181" s="2"/>
-      <c r="N181" s="7"/>
-      <c r="O181" s="7"/>
-      <c r="P181" s="7"/>
+      <c r="F181" s="8"/>
+      <c r="G181" s="8"/>
+      <c r="H181" s="8"/>
+      <c r="I181" s="8"/>
+      <c r="J181" s="8"/>
+      <c r="K181" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L181" s="8"/>
+      <c r="M181" s="9"/>
+      <c r="N181" s="8"/>
+      <c r="O181" s="8"/>
+      <c r="P181" s="8"/>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A182" s="7" t="s">
@@ -54440,11 +54980,21 @@
       <c r="E183" s="7">
         <v>486</v>
       </c>
-      <c r="F183" s="7"/>
-      <c r="G183" s="7"/>
-      <c r="H183" s="7"/>
-      <c r="I183" s="7"/>
-      <c r="J183" s="7"/>
+      <c r="F183" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G183" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H183" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I183" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J183" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K183" s="7" t="s">
         <v>7</v>
       </c>
@@ -54456,97 +55006,110 @@
       <c r="O183" s="7"/>
       <c r="P183" s="7"/>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A184" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B184" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C184" s="7">
+    <row r="184" spans="1:16" s="46" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A184" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B184" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184" s="44">
         <v>87177</v>
       </c>
-      <c r="D184" s="7">
+      <c r="D184" s="44">
         <v>87506</v>
       </c>
-      <c r="E184" s="7">
+      <c r="E184" s="44">
         <v>330</v>
       </c>
-      <c r="F184" s="7"/>
-      <c r="G184" s="7"/>
-      <c r="H184" s="7"/>
-      <c r="I184" s="7"/>
-      <c r="J184" s="7"/>
-      <c r="K184" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L184" s="7" t="s">
+      <c r="F184" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G184" s="44" t="str">
+        <f>B185</f>
+        <v>RING-finger domain-containing E3 protein CDS</v>
+      </c>
+      <c r="H184" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I184" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J184" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K184" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L184" s="44" t="s">
         <v>1307</v>
       </c>
-      <c r="M184" s="2"/>
-      <c r="N184" s="7"/>
-      <c r="O184" s="7"/>
-      <c r="P184" s="7"/>
-    </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A185" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B185" s="7" t="s">
+      <c r="M184" s="45" t="s">
+        <v>1384</v>
+      </c>
+      <c r="N184" s="44"/>
+      <c r="O184" s="44"/>
+      <c r="P184" s="44"/>
+    </row>
+    <row r="185" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B185" s="44" t="s">
         <v>1308</v>
       </c>
-      <c r="C185" s="7">
+      <c r="C185" s="44">
         <v>87177</v>
       </c>
-      <c r="D185" s="7">
+      <c r="D185" s="44">
         <v>87533</v>
       </c>
-      <c r="E185" s="7">
+      <c r="E185" s="44">
         <v>357</v>
       </c>
-      <c r="F185" s="7"/>
-      <c r="G185" s="7"/>
-      <c r="H185" s="7"/>
-      <c r="I185" s="7"/>
-      <c r="J185" s="7"/>
-      <c r="K185" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L185" s="7"/>
-      <c r="M185" s="2"/>
-      <c r="N185" s="7"/>
-      <c r="O185" s="7"/>
-      <c r="P185" s="7"/>
-    </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A186" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B186" s="7" t="s">
+      <c r="F185" s="44"/>
+      <c r="G185" s="44"/>
+      <c r="H185" s="44"/>
+      <c r="I185" s="44"/>
+      <c r="J185" s="44"/>
+      <c r="K185" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L185" s="44"/>
+      <c r="M185" s="45"/>
+      <c r="N185" s="44"/>
+      <c r="O185" s="44"/>
+      <c r="P185" s="44"/>
+    </row>
+    <row r="186" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B186" s="44" t="s">
         <v>1309</v>
       </c>
-      <c r="C186" s="7">
+      <c r="C186" s="44">
         <v>87551</v>
       </c>
-      <c r="D186" s="7">
+      <c r="D186" s="44">
         <v>88129</v>
       </c>
-      <c r="E186" s="7">
+      <c r="E186" s="44">
         <v>579</v>
       </c>
-      <c r="F186" s="7"/>
-      <c r="G186" s="7"/>
-      <c r="H186" s="7"/>
-      <c r="I186" s="7"/>
-      <c r="J186" s="7"/>
-      <c r="K186" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L186" s="7"/>
-      <c r="M186" s="2"/>
-      <c r="N186" s="7"/>
-      <c r="O186" s="7"/>
-      <c r="P186" s="7"/>
+      <c r="F186" s="44"/>
+      <c r="G186" s="44"/>
+      <c r="H186" s="44"/>
+      <c r="I186" s="44"/>
+      <c r="J186" s="44"/>
+      <c r="K186" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L186" s="44"/>
+      <c r="M186" s="45"/>
+      <c r="N186" s="44"/>
+      <c r="O186" s="44"/>
+      <c r="P186" s="44"/>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
@@ -54564,11 +55127,21 @@
       <c r="E187" s="7">
         <v>579</v>
       </c>
-      <c r="F187" s="7"/>
-      <c r="G187" s="7"/>
-      <c r="H187" s="7"/>
-      <c r="I187" s="7"/>
-      <c r="J187" s="7"/>
+      <c r="F187" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G187" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H187" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I187" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J187" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K187" s="7" t="s">
         <v>7</v>
       </c>
@@ -54626,11 +55199,21 @@
       <c r="E189" s="7">
         <v>516</v>
       </c>
-      <c r="F189" s="7"/>
-      <c r="G189" s="7"/>
-      <c r="H189" s="7"/>
-      <c r="I189" s="7"/>
-      <c r="J189" s="7"/>
+      <c r="F189" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G189" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H189" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I189" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J189" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K189" s="7" t="s">
         <v>7</v>
       </c>
@@ -54688,11 +55271,22 @@
       <c r="E191" s="7">
         <v>1431</v>
       </c>
-      <c r="F191" s="7"/>
-      <c r="G191" s="7"/>
-      <c r="H191" s="7"/>
-      <c r="I191" s="7"/>
-      <c r="J191" s="7"/>
+      <c r="F191" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G191" s="7" t="str">
+        <f>B190</f>
+        <v>ankyrin repeat-containing protein CDS</v>
+      </c>
+      <c r="H191" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I191" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J191" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K191" s="7" t="s">
         <v>9</v>
       </c>
@@ -54750,11 +55344,22 @@
       <c r="E193" s="7">
         <v>387</v>
       </c>
-      <c r="F193" s="7"/>
-      <c r="G193" s="7"/>
-      <c r="H193" s="7"/>
-      <c r="I193" s="7"/>
-      <c r="J193" s="7"/>
+      <c r="F193" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G193" s="7" t="str">
+        <f>B192</f>
+        <v>suppressor of cytokine signaling protein CDS</v>
+      </c>
+      <c r="H193" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I193" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J193" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K193" s="7" t="s">
         <v>9</v>
       </c>
@@ -54812,11 +55417,21 @@
       <c r="E195" s="7">
         <v>777</v>
       </c>
-      <c r="F195" s="7"/>
-      <c r="G195" s="7"/>
-      <c r="H195" s="7"/>
-      <c r="I195" s="7"/>
-      <c r="J195" s="7"/>
+      <c r="F195" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G195" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H195" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I195" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J195" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K195" s="7" t="s">
         <v>9</v>
       </c>
@@ -54874,11 +55489,21 @@
       <c r="E197" s="7">
         <v>372</v>
       </c>
-      <c r="F197" s="7"/>
-      <c r="G197" s="7"/>
-      <c r="H197" s="7"/>
-      <c r="I197" s="7"/>
-      <c r="J197" s="7"/>
+      <c r="F197" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G197" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H197" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I197" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J197" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K197" s="7" t="s">
         <v>9</v>
       </c>
@@ -54890,129 +55515,153 @@
       <c r="O197" s="7"/>
       <c r="P197" s="7"/>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A198" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B198" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C198" s="7">
+    <row r="198" spans="1:16" s="46" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B198" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C198" s="44">
         <v>91882</v>
       </c>
-      <c r="D198" s="7">
+      <c r="D198" s="44">
         <v>92784</v>
       </c>
-      <c r="E198" s="7">
+      <c r="E198" s="44">
         <v>903</v>
       </c>
-      <c r="F198" s="7"/>
-      <c r="G198" s="7"/>
-      <c r="H198" s="7"/>
-      <c r="I198" s="7"/>
-      <c r="J198" s="7"/>
-      <c r="K198" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L198" s="7" t="s">
+      <c r="F198" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G198" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H198" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I198" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J198" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K198" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L198" s="44" t="s">
         <v>1320</v>
       </c>
-      <c r="M198" s="2"/>
-      <c r="N198" s="7"/>
-      <c r="O198" s="7"/>
-      <c r="P198" s="7"/>
-    </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A199" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B199" s="7" t="s">
+      <c r="M198" s="45" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N198" s="44"/>
+      <c r="O198" s="44"/>
+      <c r="P198" s="44"/>
+    </row>
+    <row r="199" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B199" s="44" t="s">
         <v>1321</v>
       </c>
-      <c r="C199" s="7">
+      <c r="C199" s="44">
         <v>91882</v>
       </c>
-      <c r="D199" s="7">
+      <c r="D199" s="44">
         <v>92913</v>
       </c>
-      <c r="E199" s="7">
+      <c r="E199" s="44">
         <v>1032</v>
       </c>
-      <c r="F199" s="7"/>
-      <c r="G199" s="7"/>
-      <c r="H199" s="7"/>
-      <c r="I199" s="7"/>
-      <c r="J199" s="7"/>
-      <c r="K199" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L199" s="7"/>
-      <c r="M199" s="2"/>
-      <c r="N199" s="7"/>
-      <c r="O199" s="7"/>
-      <c r="P199" s="7"/>
-    </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A200" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B200" s="7" t="s">
+      <c r="F199" s="44"/>
+      <c r="G199" s="44"/>
+      <c r="H199" s="44"/>
+      <c r="I199" s="44"/>
+      <c r="J199" s="44"/>
+      <c r="K199" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L199" s="44"/>
+      <c r="M199" s="45"/>
+      <c r="N199" s="44"/>
+      <c r="O199" s="44"/>
+      <c r="P199" s="44"/>
+    </row>
+    <row r="200" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B200" s="44" t="s">
         <v>1322</v>
       </c>
-      <c r="C200" s="7">
+      <c r="C200" s="44">
         <v>93050</v>
       </c>
-      <c r="D200" s="7">
+      <c r="D200" s="44">
         <v>93265</v>
       </c>
-      <c r="E200" s="7">
+      <c r="E200" s="44">
         <v>216</v>
       </c>
-      <c r="F200" s="7"/>
-      <c r="G200" s="7"/>
-      <c r="H200" s="7"/>
-      <c r="I200" s="7"/>
-      <c r="J200" s="7"/>
-      <c r="K200" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L200" s="7"/>
-      <c r="M200" s="2"/>
-      <c r="N200" s="7"/>
-      <c r="O200" s="7"/>
-      <c r="P200" s="7"/>
-    </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A201" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B201" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C201" s="7">
+      <c r="F200" s="44"/>
+      <c r="G200" s="44"/>
+      <c r="H200" s="44"/>
+      <c r="I200" s="44"/>
+      <c r="J200" s="44"/>
+      <c r="K200" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L200" s="44"/>
+      <c r="M200" s="45"/>
+      <c r="N200" s="44"/>
+      <c r="O200" s="44"/>
+      <c r="P200" s="44"/>
+    </row>
+    <row r="201" spans="1:16" s="46" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A201" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B201" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C201" s="44">
         <v>92947</v>
       </c>
-      <c r="D201" s="7">
+      <c r="D201" s="44">
         <v>93549</v>
       </c>
-      <c r="E201" s="7">
+      <c r="E201" s="44">
         <v>603</v>
       </c>
-      <c r="F201" s="7"/>
-      <c r="G201" s="7"/>
-      <c r="H201" s="7"/>
-      <c r="I201" s="7"/>
-      <c r="J201" s="7"/>
-      <c r="K201" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L201" s="7" t="s">
+      <c r="F201" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G201" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="H201" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I201" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J201" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K201" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L201" s="44" t="s">
         <v>1323</v>
       </c>
-      <c r="M201" s="2"/>
-      <c r="N201" s="7"/>
-      <c r="O201" s="7"/>
-      <c r="P201" s="7"/>
+      <c r="M201" s="45" t="s">
+        <v>1386</v>
+      </c>
+      <c r="N201" s="44"/>
+      <c r="O201" s="44"/>
+      <c r="P201" s="44"/>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
@@ -55060,11 +55709,22 @@
       <c r="E203" s="7">
         <v>2763</v>
       </c>
-      <c r="F203" s="7"/>
-      <c r="G203" s="7"/>
-      <c r="H203" s="7"/>
-      <c r="I203" s="7"/>
-      <c r="J203" s="7"/>
+      <c r="F203" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G203" s="7" t="str">
+        <f>B202</f>
+        <v>D5 family NTPase CDS</v>
+      </c>
+      <c r="H203" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I203" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J203" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K203" s="7" t="s">
         <v>7</v>
       </c>
@@ -55076,67 +55736,79 @@
       <c r="O203" s="7"/>
       <c r="P203" s="7"/>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A204" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B204" s="7" t="s">
+    <row r="204" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B204" s="44" t="s">
         <v>1325</v>
       </c>
-      <c r="C204" s="7">
+      <c r="C204" s="44">
         <v>96410</v>
       </c>
-      <c r="D204" s="7">
+      <c r="D204" s="44">
         <v>96604</v>
       </c>
-      <c r="E204" s="7">
+      <c r="E204" s="44">
         <v>195</v>
       </c>
-      <c r="F204" s="7"/>
-      <c r="G204" s="7"/>
-      <c r="H204" s="7"/>
-      <c r="I204" s="7"/>
-      <c r="J204" s="7"/>
-      <c r="K204" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L204" s="7"/>
-      <c r="M204" s="2"/>
-      <c r="N204" s="7"/>
-      <c r="O204" s="7"/>
-      <c r="P204" s="7"/>
-    </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A205" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B205" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C205" s="7">
+      <c r="F204" s="44"/>
+      <c r="G204" s="44"/>
+      <c r="H204" s="44"/>
+      <c r="I204" s="44"/>
+      <c r="J204" s="44"/>
+      <c r="K204" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L204" s="44"/>
+      <c r="M204" s="45"/>
+      <c r="N204" s="44"/>
+      <c r="O204" s="44"/>
+      <c r="P204" s="44"/>
+    </row>
+    <row r="205" spans="1:16" s="46" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A205" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B205" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C205" s="44">
         <v>96449</v>
       </c>
-      <c r="D205" s="7">
+      <c r="D205" s="44">
         <v>96604</v>
       </c>
-      <c r="E205" s="7">
+      <c r="E205" s="44">
         <v>156</v>
       </c>
-      <c r="F205" s="7"/>
-      <c r="G205" s="7"/>
-      <c r="H205" s="7"/>
-      <c r="I205" s="7"/>
-      <c r="J205" s="7"/>
-      <c r="K205" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L205" s="7" t="s">
+      <c r="F205" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G205" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H205" s="47">
+        <v>96410</v>
+      </c>
+      <c r="I205" s="44">
+        <v>96604</v>
+      </c>
+      <c r="J205" s="47">
+        <v>195</v>
+      </c>
+      <c r="K205" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L205" s="44" t="s">
         <v>1326</v>
       </c>
-      <c r="M205" s="2"/>
-      <c r="N205" s="7"/>
-      <c r="O205" s="7"/>
-      <c r="P205" s="7"/>
+      <c r="M205" s="45" t="s">
+        <v>1387</v>
+      </c>
+      <c r="N205" s="44"/>
+      <c r="O205" s="44"/>
+      <c r="P205" s="44"/>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206" s="7" t="s">
@@ -55184,11 +55856,22 @@
       <c r="E207" s="7">
         <v>897</v>
       </c>
-      <c r="F207" s="7"/>
-      <c r="G207" s="7"/>
-      <c r="H207" s="7"/>
-      <c r="I207" s="7"/>
-      <c r="J207" s="7"/>
+      <c r="F207" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G207" s="7" t="str">
+        <f>B206</f>
+        <v>tumor necrosis factor type 2 receptor-associatedprotein CDS</v>
+      </c>
+      <c r="H207" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I207" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J207" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K207" s="7" t="s">
         <v>7</v>
       </c>
@@ -55246,11 +55929,22 @@
       <c r="E209" s="7">
         <v>744</v>
       </c>
-      <c r="F209" s="7"/>
-      <c r="G209" s="7"/>
-      <c r="H209" s="7"/>
-      <c r="I209" s="7"/>
-      <c r="J209" s="7"/>
+      <c r="F209" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G209" s="7" t="str">
+        <f>B208</f>
+        <v>proliferating cell nuclear antigen CDS</v>
+      </c>
+      <c r="H209" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I209" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J209" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K209" s="7" t="s">
         <v>9</v>
       </c>
@@ -55262,97 +55956,109 @@
       <c r="O209" s="7"/>
       <c r="P209" s="7"/>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A210" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B210" s="7" t="s">
+    <row r="210" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B210" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C210" s="7">
+      <c r="C210" s="44">
         <v>98369</v>
       </c>
-      <c r="D210" s="7">
+      <c r="D210" s="44">
         <v>98521</v>
       </c>
-      <c r="E210" s="7">
+      <c r="E210" s="44">
         <v>153</v>
       </c>
-      <c r="F210" s="7"/>
-      <c r="G210" s="7"/>
-      <c r="H210" s="7"/>
-      <c r="I210" s="7"/>
-      <c r="J210" s="7"/>
-      <c r="K210" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L210" s="7"/>
-      <c r="M210" s="2"/>
-      <c r="N210" s="7"/>
-      <c r="O210" s="7"/>
-      <c r="P210" s="7"/>
-    </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A211" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B211" s="7" t="s">
+      <c r="F210" s="44"/>
+      <c r="G210" s="44"/>
+      <c r="H210" s="44"/>
+      <c r="I210" s="44"/>
+      <c r="J210" s="44"/>
+      <c r="K210" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L210" s="44"/>
+      <c r="M210" s="45"/>
+      <c r="N210" s="44"/>
+      <c r="O210" s="44"/>
+      <c r="P210" s="44"/>
+    </row>
+    <row r="211" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B211" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C211" s="7">
+      <c r="C211" s="44">
         <v>98534</v>
       </c>
-      <c r="D211" s="7">
+      <c r="D211" s="44">
         <v>98749</v>
       </c>
-      <c r="E211" s="7">
+      <c r="E211" s="44">
         <v>216</v>
       </c>
-      <c r="F211" s="7"/>
-      <c r="G211" s="7"/>
-      <c r="H211" s="7"/>
-      <c r="I211" s="7"/>
-      <c r="J211" s="7"/>
-      <c r="K211" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L211" s="7"/>
-      <c r="M211" s="2"/>
-      <c r="N211" s="7"/>
-      <c r="O211" s="7"/>
-      <c r="P211" s="7"/>
-    </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A212" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B212" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C212" s="7">
+      <c r="F211" s="44"/>
+      <c r="G211" s="44"/>
+      <c r="H211" s="44"/>
+      <c r="I211" s="44"/>
+      <c r="J211" s="44"/>
+      <c r="K211" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L211" s="44"/>
+      <c r="M211" s="45"/>
+      <c r="N211" s="44"/>
+      <c r="O211" s="44"/>
+      <c r="P211" s="44"/>
+    </row>
+    <row r="212" spans="1:16" s="46" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A212" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B212" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C212" s="44">
         <v>98251</v>
       </c>
-      <c r="D212" s="7">
+      <c r="D212" s="44">
         <v>98754</v>
       </c>
-      <c r="E212" s="7">
+      <c r="E212" s="44">
         <v>504</v>
       </c>
-      <c r="F212" s="7"/>
-      <c r="G212" s="7"/>
-      <c r="H212" s="7"/>
-      <c r="I212" s="7"/>
-      <c r="J212" s="7"/>
-      <c r="K212" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L212" s="7" t="s">
+      <c r="F212" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G212" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="H212" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I212" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J212" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K212" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L212" s="44" t="s">
         <v>1330</v>
       </c>
-      <c r="M212" s="2"/>
-      <c r="N212" s="7"/>
-      <c r="O212" s="7"/>
-      <c r="P212" s="7"/>
+      <c r="M212" s="45" t="s">
+        <v>1388</v>
+      </c>
+      <c r="N212" s="44"/>
+      <c r="O212" s="44"/>
+      <c r="P212" s="44"/>
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
@@ -55384,411 +56090,501 @@
       <c r="O213" s="7"/>
       <c r="P213" s="7"/>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A214" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B214" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C214" s="7">
+    <row r="214" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B214" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C214" s="44">
         <v>98793</v>
       </c>
-      <c r="D214" s="7">
+      <c r="D214" s="44">
         <v>101375</v>
       </c>
-      <c r="E214" s="7">
+      <c r="E214" s="44">
         <v>2583</v>
       </c>
-      <c r="F214" s="7"/>
-      <c r="G214" s="7"/>
-      <c r="H214" s="7"/>
-      <c r="I214" s="7"/>
-      <c r="J214" s="7"/>
-      <c r="K214" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L214" s="7" t="s">
+      <c r="F214" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="G214" s="44" t="str">
+        <f>B213</f>
+        <v>tyrosine kinase CDS</v>
+      </c>
+      <c r="H214" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I214" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J214" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K214" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L214" s="44" t="s">
         <v>1331</v>
       </c>
-      <c r="M214" s="2"/>
-      <c r="N214" s="7"/>
-      <c r="O214" s="7"/>
-      <c r="P214" s="7"/>
-    </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A215" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B215" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C215" s="7">
+      <c r="M214" s="45"/>
+      <c r="N214" s="44"/>
+      <c r="O214" s="44"/>
+      <c r="P214" s="44"/>
+    </row>
+    <row r="215" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B215" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C215" s="44">
         <v>101484</v>
       </c>
-      <c r="D215" s="7">
+      <c r="D215" s="44">
         <v>101807</v>
       </c>
-      <c r="E215" s="7">
+      <c r="E215" s="44">
         <v>324</v>
       </c>
-      <c r="F215" s="7"/>
-      <c r="G215" s="7"/>
-      <c r="H215" s="7"/>
-      <c r="I215" s="7"/>
-      <c r="J215" s="7"/>
-      <c r="K215" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L215" s="7" t="s">
+      <c r="F215" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G215" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H215" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I215" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J215" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K215" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L215" s="44" t="s">
         <v>1332</v>
       </c>
-      <c r="M215" s="2"/>
-      <c r="N215" s="7"/>
-      <c r="O215" s="7"/>
-      <c r="P215" s="7"/>
-    </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A216" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B216" s="7" t="s">
+      <c r="M215" s="45" t="s">
+        <v>1389</v>
+      </c>
+      <c r="N215" s="44"/>
+      <c r="O215" s="44"/>
+      <c r="P215" s="44"/>
+    </row>
+    <row r="216" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B216" s="44" t="s">
         <v>1333</v>
       </c>
-      <c r="C216" s="7">
+      <c r="C216" s="44">
         <v>101972</v>
       </c>
-      <c r="D216" s="7">
+      <c r="D216" s="44">
         <v>102982</v>
       </c>
-      <c r="E216" s="7">
+      <c r="E216" s="44">
         <v>1011</v>
       </c>
-      <c r="F216" s="7"/>
-      <c r="G216" s="7"/>
-      <c r="H216" s="7"/>
-      <c r="I216" s="7"/>
-      <c r="J216" s="7"/>
-      <c r="K216" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L216" s="7"/>
-      <c r="M216" s="2"/>
-      <c r="N216" s="7"/>
-      <c r="O216" s="7"/>
-      <c r="P216" s="7"/>
-    </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A217" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B217" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C217" s="7">
+      <c r="F216" s="44"/>
+      <c r="G216" s="44"/>
+      <c r="H216" s="44"/>
+      <c r="I216" s="44"/>
+      <c r="J216" s="44"/>
+      <c r="K216" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L216" s="44"/>
+      <c r="M216" s="45"/>
+      <c r="N216" s="44"/>
+      <c r="O216" s="44"/>
+      <c r="P216" s="44"/>
+    </row>
+    <row r="217" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B217" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C217" s="44">
         <v>101972</v>
       </c>
-      <c r="D217" s="7">
+      <c r="D217" s="44">
         <v>102982</v>
       </c>
-      <c r="E217" s="7">
+      <c r="E217" s="44">
         <v>1011</v>
       </c>
-      <c r="F217" s="7"/>
-      <c r="G217" s="7"/>
-      <c r="H217" s="7"/>
-      <c r="I217" s="7"/>
-      <c r="J217" s="7"/>
-      <c r="K217" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L217" s="7" t="s">
+      <c r="F217" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="G217" s="44" t="str">
+        <f>B216</f>
+        <v>immediate early protein ICP-46 CDS</v>
+      </c>
+      <c r="H217" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I217" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J217" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K217" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L217" s="44" t="s">
         <v>1334</v>
       </c>
-      <c r="M217" s="2"/>
-      <c r="N217" s="7"/>
-      <c r="O217" s="7"/>
-      <c r="P217" s="7"/>
-    </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A218" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B218" s="7" t="s">
+      <c r="M217" s="45"/>
+      <c r="N217" s="44"/>
+      <c r="O217" s="44"/>
+      <c r="P217" s="44"/>
+    </row>
+    <row r="218" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B218" s="44" t="s">
         <v>1335</v>
       </c>
-      <c r="C218" s="7">
+      <c r="C218" s="44">
         <v>103038</v>
       </c>
-      <c r="D218" s="7">
+      <c r="D218" s="44">
         <v>104411</v>
       </c>
-      <c r="E218" s="7">
+      <c r="E218" s="44">
         <v>1374</v>
       </c>
-      <c r="F218" s="7"/>
-      <c r="G218" s="7"/>
-      <c r="H218" s="7"/>
-      <c r="I218" s="7"/>
-      <c r="J218" s="7"/>
-      <c r="K218" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L218" s="7"/>
-      <c r="M218" s="2"/>
-      <c r="N218" s="7"/>
-      <c r="O218" s="7"/>
-      <c r="P218" s="7"/>
-    </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A219" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B219" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C219" s="7">
+      <c r="F218" s="44"/>
+      <c r="G218" s="44"/>
+      <c r="H218" s="44"/>
+      <c r="I218" s="44"/>
+      <c r="J218" s="44"/>
+      <c r="K218" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L218" s="44"/>
+      <c r="M218" s="45"/>
+      <c r="N218" s="44"/>
+      <c r="O218" s="44"/>
+      <c r="P218" s="44"/>
+    </row>
+    <row r="219" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B219" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C219" s="44">
         <v>103038</v>
       </c>
-      <c r="D219" s="7">
+      <c r="D219" s="44">
         <v>104411</v>
       </c>
-      <c r="E219" s="7">
+      <c r="E219" s="44">
         <v>1374</v>
       </c>
-      <c r="F219" s="7"/>
-      <c r="G219" s="7"/>
-      <c r="H219" s="7"/>
-      <c r="I219" s="7"/>
-      <c r="J219" s="7"/>
-      <c r="K219" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L219" s="7" t="s">
+      <c r="F219" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="G219" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H219" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I219" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J219" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K219" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L219" s="44" t="s">
         <v>1336</v>
       </c>
-      <c r="M219" s="2"/>
-      <c r="N219" s="7"/>
-      <c r="O219" s="7"/>
-      <c r="P219" s="7"/>
-    </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A220" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B220" s="7" t="s">
+      <c r="M219" s="45"/>
+      <c r="N219" s="44"/>
+      <c r="O219" s="44"/>
+      <c r="P219" s="44"/>
+    </row>
+    <row r="220" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B220" s="44" t="s">
         <v>1337</v>
       </c>
-      <c r="C220" s="7">
+      <c r="C220" s="44">
         <v>104463</v>
       </c>
-      <c r="D220" s="7">
+      <c r="D220" s="44">
         <v>105137</v>
       </c>
-      <c r="E220" s="7">
+      <c r="E220" s="44">
         <v>675</v>
       </c>
-      <c r="F220" s="7"/>
-      <c r="G220" s="7"/>
-      <c r="H220" s="7"/>
-      <c r="I220" s="7"/>
-      <c r="J220" s="7"/>
-      <c r="K220" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L220" s="7"/>
-      <c r="M220" s="2"/>
-      <c r="N220" s="7"/>
-      <c r="O220" s="7"/>
-      <c r="P220" s="7"/>
-    </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A221" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B221" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C221" s="7">
+      <c r="F220" s="44"/>
+      <c r="G220" s="44"/>
+      <c r="H220" s="44"/>
+      <c r="I220" s="44"/>
+      <c r="J220" s="44"/>
+      <c r="K220" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L220" s="44"/>
+      <c r="M220" s="45"/>
+      <c r="N220" s="44"/>
+      <c r="O220" s="44"/>
+      <c r="P220" s="44"/>
+    </row>
+    <row r="221" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B221" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C221" s="44">
         <v>104463</v>
       </c>
-      <c r="D221" s="7">
+      <c r="D221" s="44">
         <v>105137</v>
       </c>
-      <c r="E221" s="7">
+      <c r="E221" s="44">
         <v>675</v>
       </c>
-      <c r="F221" s="7"/>
-      <c r="G221" s="7"/>
-      <c r="H221" s="7"/>
-      <c r="I221" s="7"/>
-      <c r="J221" s="7"/>
-      <c r="K221" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L221" s="7" t="s">
+      <c r="F221" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="G221" s="44" t="str">
+        <f>B220</f>
+        <v>early 31kDa-protein CDS</v>
+      </c>
+      <c r="H221" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I221" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J221" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K221" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L221" s="44" t="s">
         <v>1338</v>
       </c>
-      <c r="M221" s="2"/>
-      <c r="N221" s="7"/>
-      <c r="O221" s="7"/>
-      <c r="P221" s="7"/>
-    </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A222" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B222" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C222" s="7">
+      <c r="M221" s="45"/>
+      <c r="N221" s="44"/>
+      <c r="O221" s="44"/>
+      <c r="P221" s="44"/>
+    </row>
+    <row r="222" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B222" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C222" s="44">
         <v>105215</v>
       </c>
-      <c r="D222" s="7">
+      <c r="D222" s="44">
         <v>105502</v>
       </c>
-      <c r="E222" s="7">
+      <c r="E222" s="44">
         <v>288</v>
       </c>
-      <c r="F222" s="7"/>
-      <c r="G222" s="7"/>
-      <c r="H222" s="7"/>
-      <c r="I222" s="7"/>
-      <c r="J222" s="7"/>
-      <c r="K222" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L222" s="7" t="s">
+      <c r="F222" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G222" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H222" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I222" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J222" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K222" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L222" s="44" t="s">
         <v>1339</v>
       </c>
-      <c r="M222" s="2"/>
-      <c r="N222" s="7"/>
-      <c r="O222" s="7"/>
-      <c r="P222" s="7"/>
-    </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A223" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B223" s="7" t="s">
+      <c r="M222" s="45" t="s">
+        <v>1389</v>
+      </c>
+      <c r="N222" s="44"/>
+      <c r="O222" s="44"/>
+      <c r="P222" s="44"/>
+    </row>
+    <row r="223" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B223" s="44" t="s">
         <v>479</v>
       </c>
-      <c r="C223" s="7">
+      <c r="C223" s="44">
         <v>105473</v>
       </c>
-      <c r="D223" s="7">
+      <c r="D223" s="44">
         <v>106783</v>
       </c>
-      <c r="E223" s="7">
+      <c r="E223" s="44">
         <v>1311</v>
       </c>
-      <c r="F223" s="7"/>
-      <c r="G223" s="7"/>
-      <c r="H223" s="7"/>
-      <c r="I223" s="7"/>
-      <c r="J223" s="7"/>
-      <c r="K223" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L223" s="7"/>
-      <c r="M223" s="2"/>
-      <c r="N223" s="7"/>
-      <c r="O223" s="7"/>
-      <c r="P223" s="7"/>
-    </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A224" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B224" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C224" s="7">
+      <c r="F223" s="44"/>
+      <c r="G223" s="44"/>
+      <c r="H223" s="44"/>
+      <c r="I223" s="44"/>
+      <c r="J223" s="44"/>
+      <c r="K223" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L223" s="44"/>
+      <c r="M223" s="45"/>
+      <c r="N223" s="44"/>
+      <c r="O223" s="44"/>
+      <c r="P223" s="44"/>
+    </row>
+    <row r="224" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B224" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224" s="44">
         <v>105473</v>
       </c>
-      <c r="D224" s="7">
+      <c r="D224" s="44">
         <v>106783</v>
       </c>
-      <c r="E224" s="7">
+      <c r="E224" s="44">
         <v>1311</v>
       </c>
-      <c r="F224" s="7"/>
-      <c r="G224" s="7"/>
-      <c r="H224" s="7"/>
-      <c r="I224" s="7"/>
-      <c r="J224" s="7"/>
-      <c r="K224" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L224" s="7" t="s">
+      <c r="F224" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="G224" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H224" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I224" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J224" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K224" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L224" s="44" t="s">
         <v>1340</v>
       </c>
-      <c r="M224" s="2"/>
-      <c r="N224" s="7"/>
-      <c r="O224" s="7"/>
-      <c r="P224" s="7"/>
-    </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A225" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B225" s="7" t="s">
+      <c r="M224" s="45"/>
+      <c r="N224" s="44"/>
+      <c r="O224" s="44"/>
+      <c r="P224" s="44"/>
+    </row>
+    <row r="225" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B225" s="44" t="s">
         <v>1308</v>
       </c>
-      <c r="C225" s="7">
+      <c r="C225" s="44">
         <v>106777</v>
       </c>
-      <c r="D225" s="7">
+      <c r="D225" s="44">
         <v>107133</v>
       </c>
-      <c r="E225" s="7">
+      <c r="E225" s="44">
         <v>357</v>
       </c>
-      <c r="F225" s="7"/>
-      <c r="G225" s="7"/>
-      <c r="H225" s="7"/>
-      <c r="I225" s="7"/>
-      <c r="J225" s="7"/>
-      <c r="K225" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L225" s="7"/>
-      <c r="M225" s="2"/>
-      <c r="N225" s="7"/>
-      <c r="O225" s="7"/>
-      <c r="P225" s="7"/>
-    </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A226" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B226" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C226" s="7">
+      <c r="F225" s="44"/>
+      <c r="G225" s="44"/>
+      <c r="H225" s="44"/>
+      <c r="I225" s="44"/>
+      <c r="J225" s="44"/>
+      <c r="K225" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L225" s="44"/>
+      <c r="M225" s="45"/>
+      <c r="N225" s="44"/>
+      <c r="O225" s="44"/>
+      <c r="P225" s="44"/>
+    </row>
+    <row r="226" spans="1:16" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A226" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B226" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C226" s="44">
         <v>106846</v>
       </c>
-      <c r="D226" s="7">
+      <c r="D226" s="44">
         <v>107133</v>
       </c>
-      <c r="E226" s="7">
+      <c r="E226" s="44">
         <v>288</v>
       </c>
-      <c r="F226" s="7"/>
-      <c r="G226" s="7"/>
-      <c r="H226" s="7"/>
-      <c r="I226" s="7"/>
-      <c r="J226" s="7"/>
-      <c r="K226" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L226" s="7" t="s">
+      <c r="F226" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G226" s="44" t="str">
+        <f>B225</f>
+        <v>RING-finger domain-containing E3 protein CDS</v>
+      </c>
+      <c r="H226" s="47">
+        <v>106777</v>
+      </c>
+      <c r="I226" s="44">
+        <v>107133</v>
+      </c>
+      <c r="J226" s="47">
+        <v>357</v>
+      </c>
+      <c r="K226" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L226" s="44" t="s">
         <v>1341</v>
       </c>
-      <c r="M226" s="2"/>
-      <c r="N226" s="7"/>
-      <c r="O226" s="7"/>
-      <c r="P226" s="7"/>
+      <c r="M226" s="45" t="s">
+        <v>1390</v>
+      </c>
+      <c r="N226" s="44"/>
+      <c r="O226" s="44"/>
+      <c r="P226" s="44"/>
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227" s="7" t="s">
@@ -55836,11 +56632,21 @@
       <c r="E228" s="7">
         <v>507</v>
       </c>
-      <c r="F228" s="7"/>
-      <c r="G228" s="7"/>
-      <c r="H228" s="7"/>
-      <c r="I228" s="7"/>
-      <c r="J228" s="7"/>
+      <c r="F228" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G228" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H228" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I228" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J228" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K228" s="7" t="s">
         <v>9</v>
       </c>
@@ -55898,11 +56704,21 @@
       <c r="E230" s="7">
         <v>651</v>
       </c>
-      <c r="F230" s="7"/>
-      <c r="G230" s="7"/>
-      <c r="H230" s="7"/>
-      <c r="I230" s="7"/>
-      <c r="J230" s="7"/>
+      <c r="F230" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G230" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H230" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I230" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J230" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K230" s="7" t="s">
         <v>7</v>
       </c>
@@ -55960,11 +56776,21 @@
       <c r="E232" s="7">
         <v>720</v>
       </c>
-      <c r="F232" s="7"/>
-      <c r="G232" s="7"/>
-      <c r="H232" s="7"/>
-      <c r="I232" s="7"/>
-      <c r="J232" s="7"/>
+      <c r="F232" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G232" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H232" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I232" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J232" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K232" s="7" t="s">
         <v>9</v>
       </c>
@@ -55976,67 +56802,79 @@
       <c r="O232" s="7"/>
       <c r="P232" s="7"/>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A233" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B233" s="7" t="s">
+    <row r="233" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B233" s="44" t="s">
         <v>1346</v>
       </c>
-      <c r="C233" s="7">
+      <c r="C233" s="44">
         <v>109124</v>
       </c>
-      <c r="D233" s="7">
+      <c r="D233" s="44">
         <v>109318</v>
       </c>
-      <c r="E233" s="7">
+      <c r="E233" s="44">
         <v>195</v>
       </c>
-      <c r="F233" s="7"/>
-      <c r="G233" s="7"/>
-      <c r="H233" s="7"/>
-      <c r="I233" s="7"/>
-      <c r="J233" s="7"/>
-      <c r="K233" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L233" s="7"/>
-      <c r="M233" s="2"/>
-      <c r="N233" s="7"/>
-      <c r="O233" s="7"/>
-      <c r="P233" s="7"/>
-    </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A234" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B234" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C234" s="7">
+      <c r="F233" s="44"/>
+      <c r="G233" s="44"/>
+      <c r="H233" s="44"/>
+      <c r="I233" s="44"/>
+      <c r="J233" s="44"/>
+      <c r="K233" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L233" s="44"/>
+      <c r="M233" s="45"/>
+      <c r="N233" s="44"/>
+      <c r="O233" s="44"/>
+      <c r="P233" s="44"/>
+    </row>
+    <row r="234" spans="1:16" s="46" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A234" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B234" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C234" s="44">
         <v>109018</v>
       </c>
-      <c r="D234" s="7">
+      <c r="D234" s="44">
         <v>109398</v>
       </c>
-      <c r="E234" s="7">
+      <c r="E234" s="44">
         <v>381</v>
       </c>
-      <c r="F234" s="7"/>
-      <c r="G234" s="7"/>
-      <c r="H234" s="7"/>
-      <c r="I234" s="7"/>
-      <c r="J234" s="7"/>
-      <c r="K234" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L234" s="7" t="s">
+      <c r="F234" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G234" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H234" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I234" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="J234" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="K234" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L234" s="44" t="s">
         <v>1347</v>
       </c>
-      <c r="M234" s="2"/>
-      <c r="N234" s="7"/>
-      <c r="O234" s="7"/>
-      <c r="P234" s="7"/>
+      <c r="M234" s="45" t="s">
+        <v>1391</v>
+      </c>
+      <c r="N234" s="44"/>
+      <c r="O234" s="44"/>
+      <c r="P234" s="44"/>
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A235" s="7" t="s">
@@ -56054,11 +56892,22 @@
       <c r="E235" s="7">
         <v>687</v>
       </c>
-      <c r="F235" s="7"/>
-      <c r="G235" s="7"/>
-      <c r="H235" s="7"/>
-      <c r="I235" s="7"/>
-      <c r="J235" s="7"/>
+      <c r="F235" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G235" s="7" t="str">
+        <f>B236</f>
+        <v>ankyrin repeat-containing protein CDS</v>
+      </c>
+      <c r="H235" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I235" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J235" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="K235" s="7" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Updated genetic information spreadsheet when reviewing papers for phylogenetic methods used.
</commit_message>
<xml_diff>
--- a/prokka_outputs/Manually checked annotation summary/2024-08-05_Manual Check_Nucleotide alignment Annotations.xlsx
+++ b/prokka_outputs/Manually checked annotation summary/2024-08-05_Manual Check_Nucleotide alignment Annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/prokka_outputs/Manually checked annotation summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3276" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52542966-ECCA-4A27-845E-54837AB94548}"/>
+  <xr:revisionPtr revIDLastSave="3279" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5B14B51-E020-4692-8BAB-B11EE804FC30}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{2726C256-0AC9-4A8B-B368-59495ADA43C2}"/>
   </bookViews>
@@ -4235,12 +4235,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Covered the position of an annotation in the reference genome which returned 10 matches in Genbank (as opposed to 3 for the Prokka annotation). All matches for the reference egenome annotation were not equal to the size of the wuery although all matches for the reference genome annotation were. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Same numner of matches (10) of similar as matches for refrence genome annotation. Decided to keep Prokka version. </t>
-  </si>
-  <si>
     <t xml:space="preserve">One weak match in Genbank. </t>
   </si>
   <si>
@@ -4350,6 +4344,12 @@
   </si>
   <si>
     <t>More matches in GenBank for the Prokka version f this gene (as opposed to the reference genome annotation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered the position of an annotation in the reference genome which returned 10 matches in Genbank (as opposed to 3 for the Prokka annotation). All matches for the reference genome annotation were not equal to the size of the query although all matches for the reference genome annotation were. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same number of matches (10) of similar length as the matches for refrence genome annotation. Decided to keep Prokka version. </t>
   </si>
 </sst>
 </file>
@@ -4906,7 +4906,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5009,16 +5009,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -48147,8 +48137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3FEEE8-70D8-4BA8-8B68-9FBAA402446E}">
   <dimension ref="A1:P236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="C233" sqref="A233:XFD234"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48329,7 +48319,7 @@
         <v>1142</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>1353</v>
+        <v>1390</v>
       </c>
       <c r="N4" s="7"/>
       <c r="O4" s="41" t="s">
@@ -48560,7 +48550,7 @@
         <v>1148</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>1354</v>
+        <v>1391</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="41" t="s">
@@ -48990,7 +48980,7 @@
         <v>1156</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="N21" s="7"/>
       <c r="O21" s="43" t="s">
@@ -49342,7 +49332,7 @@
         <v>1164</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="N30" s="7"/>
       <c r="O30" s="41" t="s">
@@ -49420,7 +49410,7 @@
         <v>1166</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="N32" s="7"/>
       <c r="O32" s="41" t="s">
@@ -49708,7 +49698,7 @@
         <v>184</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="H40" t="s">
         <v>141</v>
@@ -49726,7 +49716,7 @@
         <v>1174</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="N40" s="7"/>
       <c r="O40" s="41" t="s">
@@ -49945,7 +49935,7 @@
         <v>1179</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="N46" s="7"/>
       <c r="O46" s="41" t="s">
@@ -50158,7 +50148,7 @@
       </c>
       <c r="L51" s="7"/>
       <c r="M51" s="26" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="N51" s="7"/>
       <c r="O51" s="43" t="s">
@@ -50619,7 +50609,7 @@
         <v>1193</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="N63" s="7"/>
       <c r="O63" s="43" t="s">
@@ -50843,7 +50833,7 @@
         <v>1199</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
@@ -51205,7 +51195,7 @@
         <v>1209</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
@@ -51321,7 +51311,7 @@
         <v>1212</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="N82" s="7"/>
       <c r="O82" s="7"/>
@@ -51901,7 +51891,7 @@
         <v>1226</v>
       </c>
       <c r="M98" s="2" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="N98" s="7"/>
       <c r="O98" s="7"/>
@@ -52119,7 +52109,7 @@
         <v>1232</v>
       </c>
       <c r="M104" s="2" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="N104" s="7"/>
       <c r="O104" s="7"/>
@@ -52413,49 +52403,49 @@
       <c r="O112" s="7"/>
       <c r="P112" s="7"/>
     </row>
-    <row r="113" spans="1:16" s="46" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B113" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C113" s="44">
+    <row r="113" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C113" s="7">
         <v>51331</v>
       </c>
-      <c r="D113" s="44">
+      <c r="D113" s="7">
         <v>51537</v>
       </c>
-      <c r="E113" s="44">
+      <c r="E113" s="7">
         <v>207</v>
       </c>
-      <c r="F113" s="44" t="s">
+      <c r="F113" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G113" s="44" t="s">
+      <c r="G113" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="H113" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I113" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J113" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K113" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L113" s="44" t="s">
+      <c r="H113" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I113" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J113" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K113" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L113" s="7" t="s">
         <v>1241</v>
       </c>
-      <c r="M113" s="45" t="s">
-        <v>1368</v>
-      </c>
-      <c r="N113" s="44"/>
-      <c r="O113" s="44"/>
-      <c r="P113" s="44"/>
+      <c r="M113" s="2" t="s">
+        <v>1366</v>
+      </c>
+      <c r="N113" s="7"/>
+      <c r="O113" s="7"/>
+      <c r="P113" s="7"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
@@ -52712,7 +52702,7 @@
         <v>1248</v>
       </c>
       <c r="M120" s="2" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="N120" s="7"/>
       <c r="O120" s="7"/>
@@ -52902,7 +52892,7 @@
         <v>1251</v>
       </c>
       <c r="M125" s="2" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="N125" s="7"/>
       <c r="O125" s="7"/>
@@ -52944,7 +52934,7 @@
       </c>
       <c r="L126" s="7"/>
       <c r="M126" s="2" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="N126" s="7"/>
       <c r="O126" s="7"/>
@@ -53073,7 +53063,7 @@
         <v>184</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="H130" s="7" t="s">
         <v>141</v>
@@ -53091,7 +53081,7 @@
         <v>1254</v>
       </c>
       <c r="M130" s="2" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="N130" s="7"/>
       <c r="O130" s="7"/>
@@ -53150,13 +53140,13 @@
         <v>178</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="I132" s="7" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="J132" s="7" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="K132" s="7" t="s">
         <v>7</v>
@@ -53237,7 +53227,7 @@
         <v>1258</v>
       </c>
       <c r="M134" s="2" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="N134" s="7"/>
       <c r="O134" s="7"/>
@@ -53383,7 +53373,7 @@
         <v>1262</v>
       </c>
       <c r="M138" s="2" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="N138" s="7"/>
       <c r="O138" s="7"/>
@@ -53487,7 +53477,7 @@
       </c>
       <c r="L141" s="7"/>
       <c r="M141" s="2" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="N141" s="7"/>
       <c r="O141" s="7"/>
@@ -53531,7 +53521,7 @@
         <v>1266</v>
       </c>
       <c r="M142" s="2" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="N142" s="7"/>
       <c r="O142" s="7"/>
@@ -53636,7 +53626,7 @@
         <v>1268</v>
       </c>
       <c r="M145" s="2" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="N145" s="7"/>
       <c r="O145" s="7"/>
@@ -53752,7 +53742,7 @@
         <v>1271</v>
       </c>
       <c r="M148" s="2" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="N148" s="7"/>
       <c r="O148" s="7"/>
@@ -54216,229 +54206,229 @@
         <v>1284</v>
       </c>
       <c r="M161" s="2" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="N161" s="7"/>
       <c r="O161" s="7"/>
       <c r="P161" s="7"/>
     </row>
-    <row r="162" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B162" s="44" t="s">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A162" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>1285</v>
       </c>
-      <c r="C162" s="44">
+      <c r="C162" s="7">
         <v>78839</v>
       </c>
-      <c r="D162" s="44">
+      <c r="D162" s="7">
         <v>79303</v>
       </c>
-      <c r="E162" s="44">
+      <c r="E162" s="7">
         <v>465</v>
       </c>
-      <c r="F162" s="44"/>
-      <c r="G162" s="44"/>
-      <c r="H162" s="44"/>
-      <c r="I162" s="44"/>
-      <c r="J162" s="44"/>
-      <c r="K162" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L162" s="44"/>
-      <c r="M162" s="45"/>
-      <c r="N162" s="44"/>
-      <c r="O162" s="44"/>
-      <c r="P162" s="44"/>
-    </row>
-    <row r="163" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B163" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C163" s="44">
+      <c r="F162" s="7"/>
+      <c r="G162" s="7"/>
+      <c r="H162" s="7"/>
+      <c r="I162" s="7"/>
+      <c r="J162" s="7"/>
+      <c r="K162" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L162" s="7"/>
+      <c r="M162" s="2"/>
+      <c r="N162" s="7"/>
+      <c r="O162" s="7"/>
+      <c r="P162" s="7"/>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A163" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C163" s="7">
         <v>78839</v>
       </c>
-      <c r="D163" s="44">
+      <c r="D163" s="7">
         <v>79303</v>
       </c>
-      <c r="E163" s="44">
+      <c r="E163" s="7">
         <v>465</v>
       </c>
-      <c r="F163" s="44" t="s">
+      <c r="F163" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G163" s="44" t="s">
+      <c r="G163" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="H163" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I163" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J163" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K163" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L163" s="44" t="s">
+      <c r="H163" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I163" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J163" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K163" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L163" s="7" t="s">
         <v>1286</v>
       </c>
-      <c r="M163" s="45"/>
-      <c r="N163" s="44"/>
-      <c r="O163" s="44"/>
-      <c r="P163" s="44"/>
-    </row>
-    <row r="164" spans="1:16" s="46" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B164" s="44" t="s">
+      <c r="M163" s="2"/>
+      <c r="N163" s="7"/>
+      <c r="O163" s="7"/>
+      <c r="P163" s="7"/>
+    </row>
+    <row r="164" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B164" s="7" t="s">
         <v>1287</v>
       </c>
-      <c r="C164" s="44">
+      <c r="C164" s="7">
         <v>79263</v>
       </c>
-      <c r="D164" s="44">
+      <c r="D164" s="7">
         <v>80066</v>
       </c>
-      <c r="E164" s="44">
+      <c r="E164" s="7">
         <v>804</v>
       </c>
-      <c r="F164" s="44"/>
-      <c r="G164" s="44"/>
-      <c r="H164" s="44"/>
-      <c r="I164" s="44"/>
-      <c r="J164" s="44"/>
-      <c r="K164" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L164" s="44"/>
-      <c r="M164" s="45"/>
-      <c r="N164" s="44"/>
-      <c r="O164" s="44"/>
-      <c r="P164" s="44"/>
-    </row>
-    <row r="165" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B165" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C165" s="44">
+      <c r="F164" s="7"/>
+      <c r="G164" s="7"/>
+      <c r="H164" s="7"/>
+      <c r="I164" s="7"/>
+      <c r="J164" s="7"/>
+      <c r="K164" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L164" s="7"/>
+      <c r="M164" s="2"/>
+      <c r="N164" s="7"/>
+      <c r="O164" s="7"/>
+      <c r="P164" s="7"/>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A165" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C165" s="7">
         <v>79296</v>
       </c>
-      <c r="D165" s="44">
+      <c r="D165" s="7">
         <v>80066</v>
       </c>
-      <c r="E165" s="44">
+      <c r="E165" s="7">
         <v>771</v>
       </c>
-      <c r="F165" s="44" t="s">
+      <c r="F165" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G165" s="44" t="s">
+      <c r="G165" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="H165" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I165" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J165" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K165" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L165" s="44" t="s">
+      <c r="H165" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I165" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J165" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K165" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L165" s="7" t="s">
         <v>1288</v>
       </c>
-      <c r="M165" s="45"/>
-      <c r="N165" s="44"/>
-      <c r="O165" s="44"/>
-      <c r="P165" s="44"/>
-    </row>
-    <row r="166" spans="1:16" s="46" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A166" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B166" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C166" s="44">
+      <c r="M165" s="2"/>
+      <c r="N165" s="7"/>
+      <c r="O165" s="7"/>
+      <c r="P165" s="7"/>
+    </row>
+    <row r="166" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A166" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C166" s="7">
         <v>80063</v>
       </c>
-      <c r="D166" s="44">
+      <c r="D166" s="7">
         <v>80476</v>
       </c>
-      <c r="E166" s="44">
+      <c r="E166" s="7">
         <v>414</v>
       </c>
-      <c r="F166" s="44" t="s">
+      <c r="F166" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G166" s="44" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H166" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I166" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J166" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K166" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L166" s="44" t="s">
+      <c r="G166" s="7" t="s">
+        <v>1380</v>
+      </c>
+      <c r="H166" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I166" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J166" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K166" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L166" s="7" t="s">
         <v>1289</v>
       </c>
-      <c r="M166" s="45" t="s">
-        <v>1383</v>
-      </c>
-      <c r="N166" s="44"/>
-      <c r="O166" s="44"/>
-      <c r="P166" s="44"/>
-    </row>
-    <row r="167" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B167" s="44" t="s">
+      <c r="M166" s="2" t="s">
+        <v>1381</v>
+      </c>
+      <c r="N166" s="7"/>
+      <c r="O166" s="7"/>
+      <c r="P166" s="7"/>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A167" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B167" s="7" t="s">
         <v>1290</v>
       </c>
-      <c r="C167" s="44">
+      <c r="C167" s="7">
         <v>80256</v>
       </c>
-      <c r="D167" s="44">
+      <c r="D167" s="7">
         <v>80573</v>
       </c>
-      <c r="E167" s="44">
+      <c r="E167" s="7">
         <v>318</v>
       </c>
-      <c r="F167" s="44"/>
-      <c r="G167" s="44"/>
-      <c r="H167" s="44"/>
-      <c r="I167" s="44"/>
-      <c r="J167" s="44"/>
-      <c r="K167" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L167" s="44"/>
-      <c r="M167" s="45"/>
-      <c r="N167" s="44"/>
-      <c r="O167" s="44"/>
-      <c r="P167" s="44"/>
+      <c r="F167" s="7"/>
+      <c r="G167" s="7"/>
+      <c r="H167" s="7"/>
+      <c r="I167" s="7"/>
+      <c r="J167" s="7"/>
+      <c r="K167" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L167" s="7"/>
+      <c r="M167" s="2"/>
+      <c r="N167" s="7"/>
+      <c r="O167" s="7"/>
+      <c r="P167" s="7"/>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168" s="7" t="s">
@@ -54584,77 +54574,77 @@
       <c r="O171" s="7"/>
       <c r="P171" s="7"/>
     </row>
-    <row r="172" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B172" s="44" t="s">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A172" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B172" s="7" t="s">
         <v>1295</v>
       </c>
-      <c r="C172" s="44">
+      <c r="C172" s="7">
         <v>83094</v>
       </c>
-      <c r="D172" s="44">
+      <c r="D172" s="7">
         <v>83273</v>
       </c>
-      <c r="E172" s="44">
+      <c r="E172" s="7">
         <v>180</v>
       </c>
-      <c r="F172" s="44"/>
-      <c r="G172" s="44"/>
-      <c r="H172" s="44"/>
-      <c r="I172" s="44"/>
-      <c r="J172" s="44"/>
-      <c r="K172" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L172" s="44"/>
-      <c r="M172" s="45"/>
-      <c r="N172" s="44"/>
-      <c r="O172" s="44"/>
-      <c r="P172" s="44"/>
-    </row>
-    <row r="173" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B173" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C173" s="44">
+      <c r="F172" s="7"/>
+      <c r="G172" s="7"/>
+      <c r="H172" s="7"/>
+      <c r="I172" s="7"/>
+      <c r="J172" s="7"/>
+      <c r="K172" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L172" s="7"/>
+      <c r="M172" s="2"/>
+      <c r="N172" s="7"/>
+      <c r="O172" s="7"/>
+      <c r="P172" s="7"/>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A173" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" s="7">
         <v>83103</v>
       </c>
-      <c r="D173" s="44">
+      <c r="D173" s="7">
         <v>83273</v>
       </c>
-      <c r="E173" s="44">
+      <c r="E173" s="7">
         <v>171</v>
       </c>
-      <c r="F173" s="44" t="s">
+      <c r="F173" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G173" s="44" t="s">
+      <c r="G173" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H173" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I173" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J173" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K173" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L173" s="44" t="s">
+      <c r="H173" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I173" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J173" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K173" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L173" s="7" t="s">
         <v>1296</v>
       </c>
-      <c r="M173" s="45"/>
-      <c r="N173" s="44"/>
-      <c r="O173" s="44"/>
-      <c r="P173" s="44"/>
+      <c r="M173" s="2"/>
+      <c r="N173" s="7"/>
+      <c r="O173" s="7"/>
+      <c r="P173" s="7"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
@@ -55006,110 +54996,110 @@
       <c r="O183" s="7"/>
       <c r="P183" s="7"/>
     </row>
-    <row r="184" spans="1:16" s="46" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A184" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B184" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C184" s="44">
+    <row r="184" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A184" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184" s="7">
         <v>87177</v>
       </c>
-      <c r="D184" s="44">
+      <c r="D184" s="7">
         <v>87506</v>
       </c>
-      <c r="E184" s="44">
+      <c r="E184" s="7">
         <v>330</v>
       </c>
-      <c r="F184" s="44" t="s">
+      <c r="F184" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G184" s="44" t="str">
+      <c r="G184" s="7" t="str">
         <f>B185</f>
         <v>RING-finger domain-containing E3 protein CDS</v>
       </c>
-      <c r="H184" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I184" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J184" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K184" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L184" s="44" t="s">
+      <c r="H184" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I184" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J184" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K184" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L184" s="7" t="s">
         <v>1307</v>
       </c>
-      <c r="M184" s="45" t="s">
-        <v>1384</v>
-      </c>
-      <c r="N184" s="44"/>
-      <c r="O184" s="44"/>
-      <c r="P184" s="44"/>
-    </row>
-    <row r="185" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B185" s="44" t="s">
+      <c r="M184" s="2" t="s">
+        <v>1382</v>
+      </c>
+      <c r="N184" s="7"/>
+      <c r="O184" s="7"/>
+      <c r="P184" s="7"/>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A185" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B185" s="7" t="s">
         <v>1308</v>
       </c>
-      <c r="C185" s="44">
+      <c r="C185" s="7">
         <v>87177</v>
       </c>
-      <c r="D185" s="44">
+      <c r="D185" s="7">
         <v>87533</v>
       </c>
-      <c r="E185" s="44">
+      <c r="E185" s="7">
         <v>357</v>
       </c>
-      <c r="F185" s="44"/>
-      <c r="G185" s="44"/>
-      <c r="H185" s="44"/>
-      <c r="I185" s="44"/>
-      <c r="J185" s="44"/>
-      <c r="K185" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L185" s="44"/>
-      <c r="M185" s="45"/>
-      <c r="N185" s="44"/>
-      <c r="O185" s="44"/>
-      <c r="P185" s="44"/>
-    </row>
-    <row r="186" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B186" s="44" t="s">
+      <c r="F185" s="7"/>
+      <c r="G185" s="7"/>
+      <c r="H185" s="7"/>
+      <c r="I185" s="7"/>
+      <c r="J185" s="7"/>
+      <c r="K185" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L185" s="7"/>
+      <c r="M185" s="2"/>
+      <c r="N185" s="7"/>
+      <c r="O185" s="7"/>
+      <c r="P185" s="7"/>
+    </row>
+    <row r="186" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A186" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B186" s="7" t="s">
         <v>1309</v>
       </c>
-      <c r="C186" s="44">
+      <c r="C186" s="7">
         <v>87551</v>
       </c>
-      <c r="D186" s="44">
+      <c r="D186" s="7">
         <v>88129</v>
       </c>
-      <c r="E186" s="44">
+      <c r="E186" s="7">
         <v>579</v>
       </c>
-      <c r="F186" s="44"/>
-      <c r="G186" s="44"/>
-      <c r="H186" s="44"/>
-      <c r="I186" s="44"/>
-      <c r="J186" s="44"/>
-      <c r="K186" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L186" s="44"/>
-      <c r="M186" s="45"/>
-      <c r="N186" s="44"/>
-      <c r="O186" s="44"/>
-      <c r="P186" s="44"/>
+      <c r="F186" s="7"/>
+      <c r="G186" s="7"/>
+      <c r="H186" s="7"/>
+      <c r="I186" s="7"/>
+      <c r="J186" s="7"/>
+      <c r="K186" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L186" s="7"/>
+      <c r="M186" s="2"/>
+      <c r="N186" s="7"/>
+      <c r="O186" s="7"/>
+      <c r="P186" s="7"/>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
@@ -55515,153 +55505,153 @@
       <c r="O197" s="7"/>
       <c r="P197" s="7"/>
     </row>
-    <row r="198" spans="1:16" s="46" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B198" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C198" s="44">
+    <row r="198" spans="1:16" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C198" s="7">
         <v>91882</v>
       </c>
-      <c r="D198" s="44">
+      <c r="D198" s="7">
         <v>92784</v>
       </c>
-      <c r="E198" s="44">
+      <c r="E198" s="7">
         <v>903</v>
       </c>
-      <c r="F198" s="44" t="s">
+      <c r="F198" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G198" s="44" t="s">
+      <c r="G198" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H198" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I198" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J198" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K198" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L198" s="44" t="s">
+      <c r="H198" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I198" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J198" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K198" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L198" s="7" t="s">
         <v>1320</v>
       </c>
-      <c r="M198" s="45" t="s">
-        <v>1385</v>
-      </c>
-      <c r="N198" s="44"/>
-      <c r="O198" s="44"/>
-      <c r="P198" s="44"/>
-    </row>
-    <row r="199" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B199" s="44" t="s">
+      <c r="M198" s="2" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N198" s="7"/>
+      <c r="O198" s="7"/>
+      <c r="P198" s="7"/>
+    </row>
+    <row r="199" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A199" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B199" s="7" t="s">
         <v>1321</v>
       </c>
-      <c r="C199" s="44">
+      <c r="C199" s="7">
         <v>91882</v>
       </c>
-      <c r="D199" s="44">
+      <c r="D199" s="7">
         <v>92913</v>
       </c>
-      <c r="E199" s="44">
+      <c r="E199" s="7">
         <v>1032</v>
       </c>
-      <c r="F199" s="44"/>
-      <c r="G199" s="44"/>
-      <c r="H199" s="44"/>
-      <c r="I199" s="44"/>
-      <c r="J199" s="44"/>
-      <c r="K199" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L199" s="44"/>
-      <c r="M199" s="45"/>
-      <c r="N199" s="44"/>
-      <c r="O199" s="44"/>
-      <c r="P199" s="44"/>
-    </row>
-    <row r="200" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B200" s="44" t="s">
+      <c r="F199" s="7"/>
+      <c r="G199" s="7"/>
+      <c r="H199" s="7"/>
+      <c r="I199" s="7"/>
+      <c r="J199" s="7"/>
+      <c r="K199" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L199" s="7"/>
+      <c r="M199" s="2"/>
+      <c r="N199" s="7"/>
+      <c r="O199" s="7"/>
+      <c r="P199" s="7"/>
+    </row>
+    <row r="200" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A200" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B200" s="7" t="s">
         <v>1322</v>
       </c>
-      <c r="C200" s="44">
+      <c r="C200" s="7">
         <v>93050</v>
       </c>
-      <c r="D200" s="44">
+      <c r="D200" s="7">
         <v>93265</v>
       </c>
-      <c r="E200" s="44">
+      <c r="E200" s="7">
         <v>216</v>
       </c>
-      <c r="F200" s="44"/>
-      <c r="G200" s="44"/>
-      <c r="H200" s="44"/>
-      <c r="I200" s="44"/>
-      <c r="J200" s="44"/>
-      <c r="K200" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L200" s="44"/>
-      <c r="M200" s="45"/>
-      <c r="N200" s="44"/>
-      <c r="O200" s="44"/>
-      <c r="P200" s="44"/>
-    </row>
-    <row r="201" spans="1:16" s="46" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A201" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B201" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C201" s="44">
+      <c r="F200" s="7"/>
+      <c r="G200" s="7"/>
+      <c r="H200" s="7"/>
+      <c r="I200" s="7"/>
+      <c r="J200" s="7"/>
+      <c r="K200" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L200" s="7"/>
+      <c r="M200" s="2"/>
+      <c r="N200" s="7"/>
+      <c r="O200" s="7"/>
+      <c r="P200" s="7"/>
+    </row>
+    <row r="201" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A201" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C201" s="7">
         <v>92947</v>
       </c>
-      <c r="D201" s="44">
+      <c r="D201" s="7">
         <v>93549</v>
       </c>
-      <c r="E201" s="44">
+      <c r="E201" s="7">
         <v>603</v>
       </c>
-      <c r="F201" s="44" t="s">
+      <c r="F201" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G201" s="44" t="s">
+      <c r="G201" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="H201" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I201" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J201" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K201" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L201" s="44" t="s">
+      <c r="H201" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I201" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J201" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K201" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L201" s="7" t="s">
         <v>1323</v>
       </c>
-      <c r="M201" s="45" t="s">
-        <v>1386</v>
-      </c>
-      <c r="N201" s="44"/>
-      <c r="O201" s="44"/>
-      <c r="P201" s="44"/>
+      <c r="M201" s="2" t="s">
+        <v>1384</v>
+      </c>
+      <c r="N201" s="7"/>
+      <c r="O201" s="7"/>
+      <c r="P201" s="7"/>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
@@ -55736,79 +55726,79 @@
       <c r="O203" s="7"/>
       <c r="P203" s="7"/>
     </row>
-    <row r="204" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B204" s="44" t="s">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A204" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B204" s="7" t="s">
         <v>1325</v>
       </c>
-      <c r="C204" s="44">
+      <c r="C204" s="7">
         <v>96410</v>
       </c>
-      <c r="D204" s="44">
+      <c r="D204" s="7">
         <v>96604</v>
       </c>
-      <c r="E204" s="44">
+      <c r="E204" s="7">
         <v>195</v>
       </c>
-      <c r="F204" s="44"/>
-      <c r="G204" s="44"/>
-      <c r="H204" s="44"/>
-      <c r="I204" s="44"/>
-      <c r="J204" s="44"/>
-      <c r="K204" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L204" s="44"/>
-      <c r="M204" s="45"/>
-      <c r="N204" s="44"/>
-      <c r="O204" s="44"/>
-      <c r="P204" s="44"/>
-    </row>
-    <row r="205" spans="1:16" s="46" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A205" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B205" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C205" s="44">
+      <c r="F204" s="7"/>
+      <c r="G204" s="7"/>
+      <c r="H204" s="7"/>
+      <c r="I204" s="7"/>
+      <c r="J204" s="7"/>
+      <c r="K204" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L204" s="7"/>
+      <c r="M204" s="2"/>
+      <c r="N204" s="7"/>
+      <c r="O204" s="7"/>
+      <c r="P204" s="7"/>
+    </row>
+    <row r="205" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A205" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B205" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C205" s="7">
         <v>96449</v>
       </c>
-      <c r="D205" s="44">
+      <c r="D205" s="7">
         <v>96604</v>
       </c>
-      <c r="E205" s="44">
+      <c r="E205" s="7">
         <v>156</v>
       </c>
-      <c r="F205" s="44" t="s">
+      <c r="F205" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G205" s="44" t="s">
+      <c r="G205" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H205" s="47">
+      <c r="H205" s="11">
         <v>96410</v>
       </c>
-      <c r="I205" s="44">
+      <c r="I205" s="7">
         <v>96604</v>
       </c>
-      <c r="J205" s="47">
+      <c r="J205" s="11">
         <v>195</v>
       </c>
-      <c r="K205" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L205" s="44" t="s">
+      <c r="K205" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L205" s="7" t="s">
         <v>1326</v>
       </c>
-      <c r="M205" s="45" t="s">
-        <v>1387</v>
-      </c>
-      <c r="N205" s="44"/>
-      <c r="O205" s="44"/>
-      <c r="P205" s="44"/>
+      <c r="M205" s="2" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N205" s="7"/>
+      <c r="O205" s="7"/>
+      <c r="P205" s="7"/>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206" s="7" t="s">
@@ -55956,109 +55946,109 @@
       <c r="O209" s="7"/>
       <c r="P209" s="7"/>
     </row>
-    <row r="210" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B210" s="44" t="s">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A210" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B210" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C210" s="44">
+      <c r="C210" s="7">
         <v>98369</v>
       </c>
-      <c r="D210" s="44">
+      <c r="D210" s="7">
         <v>98521</v>
       </c>
-      <c r="E210" s="44">
+      <c r="E210" s="7">
         <v>153</v>
       </c>
-      <c r="F210" s="44"/>
-      <c r="G210" s="44"/>
-      <c r="H210" s="44"/>
-      <c r="I210" s="44"/>
-      <c r="J210" s="44"/>
-      <c r="K210" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L210" s="44"/>
-      <c r="M210" s="45"/>
-      <c r="N210" s="44"/>
-      <c r="O210" s="44"/>
-      <c r="P210" s="44"/>
-    </row>
-    <row r="211" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B211" s="44" t="s">
+      <c r="F210" s="7"/>
+      <c r="G210" s="7"/>
+      <c r="H210" s="7"/>
+      <c r="I210" s="7"/>
+      <c r="J210" s="7"/>
+      <c r="K210" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L210" s="7"/>
+      <c r="M210" s="2"/>
+      <c r="N210" s="7"/>
+      <c r="O210" s="7"/>
+      <c r="P210" s="7"/>
+    </row>
+    <row r="211" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A211" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B211" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C211" s="44">
+      <c r="C211" s="7">
         <v>98534</v>
       </c>
-      <c r="D211" s="44">
+      <c r="D211" s="7">
         <v>98749</v>
       </c>
-      <c r="E211" s="44">
+      <c r="E211" s="7">
         <v>216</v>
       </c>
-      <c r="F211" s="44"/>
-      <c r="G211" s="44"/>
-      <c r="H211" s="44"/>
-      <c r="I211" s="44"/>
-      <c r="J211" s="44"/>
-      <c r="K211" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L211" s="44"/>
-      <c r="M211" s="45"/>
-      <c r="N211" s="44"/>
-      <c r="O211" s="44"/>
-      <c r="P211" s="44"/>
-    </row>
-    <row r="212" spans="1:16" s="46" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A212" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B212" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C212" s="44">
+      <c r="F211" s="7"/>
+      <c r="G211" s="7"/>
+      <c r="H211" s="7"/>
+      <c r="I211" s="7"/>
+      <c r="J211" s="7"/>
+      <c r="K211" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L211" s="7"/>
+      <c r="M211" s="2"/>
+      <c r="N211" s="7"/>
+      <c r="O211" s="7"/>
+      <c r="P211" s="7"/>
+    </row>
+    <row r="212" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A212" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C212" s="7">
         <v>98251</v>
       </c>
-      <c r="D212" s="44">
+      <c r="D212" s="7">
         <v>98754</v>
       </c>
-      <c r="E212" s="44">
+      <c r="E212" s="7">
         <v>504</v>
       </c>
-      <c r="F212" s="44" t="s">
+      <c r="F212" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G212" s="44" t="s">
+      <c r="G212" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="H212" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I212" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J212" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K212" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L212" s="44" t="s">
+      <c r="H212" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I212" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J212" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K212" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L212" s="7" t="s">
         <v>1330</v>
       </c>
-      <c r="M212" s="45" t="s">
-        <v>1388</v>
-      </c>
-      <c r="N212" s="44"/>
-      <c r="O212" s="44"/>
-      <c r="P212" s="44"/>
+      <c r="M212" s="2" t="s">
+        <v>1386</v>
+      </c>
+      <c r="N212" s="7"/>
+      <c r="O212" s="7"/>
+      <c r="P212" s="7"/>
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
@@ -56090,501 +56080,501 @@
       <c r="O213" s="7"/>
       <c r="P213" s="7"/>
     </row>
-    <row r="214" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B214" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C214" s="44">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A214" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B214" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C214" s="7">
         <v>98793</v>
       </c>
-      <c r="D214" s="44">
+      <c r="D214" s="7">
         <v>101375</v>
       </c>
-      <c r="E214" s="44">
+      <c r="E214" s="7">
         <v>2583</v>
       </c>
-      <c r="F214" s="44" t="s">
+      <c r="F214" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G214" s="44" t="str">
+      <c r="G214" s="7" t="str">
         <f>B213</f>
         <v>tyrosine kinase CDS</v>
       </c>
-      <c r="H214" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I214" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J214" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K214" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L214" s="44" t="s">
+      <c r="H214" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I214" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J214" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K214" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L214" s="7" t="s">
         <v>1331</v>
       </c>
-      <c r="M214" s="45"/>
-      <c r="N214" s="44"/>
-      <c r="O214" s="44"/>
-      <c r="P214" s="44"/>
-    </row>
-    <row r="215" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B215" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C215" s="44">
+      <c r="M214" s="2"/>
+      <c r="N214" s="7"/>
+      <c r="O214" s="7"/>
+      <c r="P214" s="7"/>
+    </row>
+    <row r="215" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A215" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B215" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C215" s="7">
         <v>101484</v>
       </c>
-      <c r="D215" s="44">
+      <c r="D215" s="7">
         <v>101807</v>
       </c>
-      <c r="E215" s="44">
+      <c r="E215" s="7">
         <v>324</v>
       </c>
-      <c r="F215" s="44" t="s">
+      <c r="F215" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G215" s="44" t="s">
+      <c r="G215" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H215" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I215" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J215" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K215" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L215" s="44" t="s">
+      <c r="H215" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I215" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J215" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K215" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L215" s="7" t="s">
         <v>1332</v>
       </c>
-      <c r="M215" s="45" t="s">
-        <v>1389</v>
-      </c>
-      <c r="N215" s="44"/>
-      <c r="O215" s="44"/>
-      <c r="P215" s="44"/>
-    </row>
-    <row r="216" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B216" s="44" t="s">
+      <c r="M215" s="2" t="s">
+        <v>1387</v>
+      </c>
+      <c r="N215" s="7"/>
+      <c r="O215" s="7"/>
+      <c r="P215" s="7"/>
+    </row>
+    <row r="216" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A216" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B216" s="7" t="s">
         <v>1333</v>
       </c>
-      <c r="C216" s="44">
+      <c r="C216" s="7">
         <v>101972</v>
       </c>
-      <c r="D216" s="44">
+      <c r="D216" s="7">
         <v>102982</v>
       </c>
-      <c r="E216" s="44">
+      <c r="E216" s="7">
         <v>1011</v>
       </c>
-      <c r="F216" s="44"/>
-      <c r="G216" s="44"/>
-      <c r="H216" s="44"/>
-      <c r="I216" s="44"/>
-      <c r="J216" s="44"/>
-      <c r="K216" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L216" s="44"/>
-      <c r="M216" s="45"/>
-      <c r="N216" s="44"/>
-      <c r="O216" s="44"/>
-      <c r="P216" s="44"/>
-    </row>
-    <row r="217" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B217" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C217" s="44">
+      <c r="F216" s="7"/>
+      <c r="G216" s="7"/>
+      <c r="H216" s="7"/>
+      <c r="I216" s="7"/>
+      <c r="J216" s="7"/>
+      <c r="K216" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L216" s="7"/>
+      <c r="M216" s="2"/>
+      <c r="N216" s="7"/>
+      <c r="O216" s="7"/>
+      <c r="P216" s="7"/>
+    </row>
+    <row r="217" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A217" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B217" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C217" s="7">
         <v>101972</v>
       </c>
-      <c r="D217" s="44">
+      <c r="D217" s="7">
         <v>102982</v>
       </c>
-      <c r="E217" s="44">
+      <c r="E217" s="7">
         <v>1011</v>
       </c>
-      <c r="F217" s="44" t="s">
+      <c r="F217" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G217" s="44" t="str">
+      <c r="G217" s="7" t="str">
         <f>B216</f>
         <v>immediate early protein ICP-46 CDS</v>
       </c>
-      <c r="H217" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I217" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J217" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K217" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L217" s="44" t="s">
+      <c r="H217" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I217" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J217" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K217" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L217" s="7" t="s">
         <v>1334</v>
       </c>
-      <c r="M217" s="45"/>
-      <c r="N217" s="44"/>
-      <c r="O217" s="44"/>
-      <c r="P217" s="44"/>
-    </row>
-    <row r="218" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B218" s="44" t="s">
+      <c r="M217" s="2"/>
+      <c r="N217" s="7"/>
+      <c r="O217" s="7"/>
+      <c r="P217" s="7"/>
+    </row>
+    <row r="218" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A218" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B218" s="7" t="s">
         <v>1335</v>
       </c>
-      <c r="C218" s="44">
+      <c r="C218" s="7">
         <v>103038</v>
       </c>
-      <c r="D218" s="44">
+      <c r="D218" s="7">
         <v>104411</v>
       </c>
-      <c r="E218" s="44">
+      <c r="E218" s="7">
         <v>1374</v>
       </c>
-      <c r="F218" s="44"/>
-      <c r="G218" s="44"/>
-      <c r="H218" s="44"/>
-      <c r="I218" s="44"/>
-      <c r="J218" s="44"/>
-      <c r="K218" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L218" s="44"/>
-      <c r="M218" s="45"/>
-      <c r="N218" s="44"/>
-      <c r="O218" s="44"/>
-      <c r="P218" s="44"/>
-    </row>
-    <row r="219" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B219" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C219" s="44">
+      <c r="F218" s="7"/>
+      <c r="G218" s="7"/>
+      <c r="H218" s="7"/>
+      <c r="I218" s="7"/>
+      <c r="J218" s="7"/>
+      <c r="K218" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L218" s="7"/>
+      <c r="M218" s="2"/>
+      <c r="N218" s="7"/>
+      <c r="O218" s="7"/>
+      <c r="P218" s="7"/>
+    </row>
+    <row r="219" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A219" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B219" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C219" s="7">
         <v>103038</v>
       </c>
-      <c r="D219" s="44">
+      <c r="D219" s="7">
         <v>104411</v>
       </c>
-      <c r="E219" s="44">
+      <c r="E219" s="7">
         <v>1374</v>
       </c>
-      <c r="F219" s="44" t="s">
+      <c r="F219" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G219" s="44" t="s">
+      <c r="G219" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H219" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I219" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J219" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K219" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L219" s="44" t="s">
+      <c r="H219" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I219" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J219" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K219" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L219" s="7" t="s">
         <v>1336</v>
       </c>
-      <c r="M219" s="45"/>
-      <c r="N219" s="44"/>
-      <c r="O219" s="44"/>
-      <c r="P219" s="44"/>
-    </row>
-    <row r="220" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B220" s="44" t="s">
+      <c r="M219" s="2"/>
+      <c r="N219" s="7"/>
+      <c r="O219" s="7"/>
+      <c r="P219" s="7"/>
+    </row>
+    <row r="220" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A220" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B220" s="7" t="s">
         <v>1337</v>
       </c>
-      <c r="C220" s="44">
+      <c r="C220" s="7">
         <v>104463</v>
       </c>
-      <c r="D220" s="44">
+      <c r="D220" s="7">
         <v>105137</v>
       </c>
-      <c r="E220" s="44">
+      <c r="E220" s="7">
         <v>675</v>
       </c>
-      <c r="F220" s="44"/>
-      <c r="G220" s="44"/>
-      <c r="H220" s="44"/>
-      <c r="I220" s="44"/>
-      <c r="J220" s="44"/>
-      <c r="K220" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L220" s="44"/>
-      <c r="M220" s="45"/>
-      <c r="N220" s="44"/>
-      <c r="O220" s="44"/>
-      <c r="P220" s="44"/>
-    </row>
-    <row r="221" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B221" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C221" s="44">
+      <c r="F220" s="7"/>
+      <c r="G220" s="7"/>
+      <c r="H220" s="7"/>
+      <c r="I220" s="7"/>
+      <c r="J220" s="7"/>
+      <c r="K220" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L220" s="7"/>
+      <c r="M220" s="2"/>
+      <c r="N220" s="7"/>
+      <c r="O220" s="7"/>
+      <c r="P220" s="7"/>
+    </row>
+    <row r="221" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A221" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B221" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C221" s="7">
         <v>104463</v>
       </c>
-      <c r="D221" s="44">
+      <c r="D221" s="7">
         <v>105137</v>
       </c>
-      <c r="E221" s="44">
+      <c r="E221" s="7">
         <v>675</v>
       </c>
-      <c r="F221" s="44" t="s">
+      <c r="F221" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G221" s="44" t="str">
+      <c r="G221" s="7" t="str">
         <f>B220</f>
         <v>early 31kDa-protein CDS</v>
       </c>
-      <c r="H221" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I221" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J221" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K221" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L221" s="44" t="s">
+      <c r="H221" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I221" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J221" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K221" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L221" s="7" t="s">
         <v>1338</v>
       </c>
-      <c r="M221" s="45"/>
-      <c r="N221" s="44"/>
-      <c r="O221" s="44"/>
-      <c r="P221" s="44"/>
-    </row>
-    <row r="222" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B222" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C222" s="44">
+      <c r="M221" s="2"/>
+      <c r="N221" s="7"/>
+      <c r="O221" s="7"/>
+      <c r="P221" s="7"/>
+    </row>
+    <row r="222" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A222" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B222" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C222" s="7">
         <v>105215</v>
       </c>
-      <c r="D222" s="44">
+      <c r="D222" s="7">
         <v>105502</v>
       </c>
-      <c r="E222" s="44">
+      <c r="E222" s="7">
         <v>288</v>
       </c>
-      <c r="F222" s="44" t="s">
+      <c r="F222" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G222" s="44" t="s">
+      <c r="G222" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H222" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I222" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J222" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K222" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L222" s="44" t="s">
+      <c r="H222" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I222" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J222" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K222" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L222" s="7" t="s">
         <v>1339</v>
       </c>
-      <c r="M222" s="45" t="s">
-        <v>1389</v>
-      </c>
-      <c r="N222" s="44"/>
-      <c r="O222" s="44"/>
-      <c r="P222" s="44"/>
-    </row>
-    <row r="223" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B223" s="44" t="s">
+      <c r="M222" s="2" t="s">
+        <v>1387</v>
+      </c>
+      <c r="N222" s="7"/>
+      <c r="O222" s="7"/>
+      <c r="P222" s="7"/>
+    </row>
+    <row r="223" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A223" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B223" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="C223" s="44">
+      <c r="C223" s="7">
         <v>105473</v>
       </c>
-      <c r="D223" s="44">
+      <c r="D223" s="7">
         <v>106783</v>
       </c>
-      <c r="E223" s="44">
+      <c r="E223" s="7">
         <v>1311</v>
       </c>
-      <c r="F223" s="44"/>
-      <c r="G223" s="44"/>
-      <c r="H223" s="44"/>
-      <c r="I223" s="44"/>
-      <c r="J223" s="44"/>
-      <c r="K223" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L223" s="44"/>
-      <c r="M223" s="45"/>
-      <c r="N223" s="44"/>
-      <c r="O223" s="44"/>
-      <c r="P223" s="44"/>
-    </row>
-    <row r="224" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B224" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C224" s="44">
+      <c r="F223" s="7"/>
+      <c r="G223" s="7"/>
+      <c r="H223" s="7"/>
+      <c r="I223" s="7"/>
+      <c r="J223" s="7"/>
+      <c r="K223" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L223" s="7"/>
+      <c r="M223" s="2"/>
+      <c r="N223" s="7"/>
+      <c r="O223" s="7"/>
+      <c r="P223" s="7"/>
+    </row>
+    <row r="224" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A224" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B224" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224" s="7">
         <v>105473</v>
       </c>
-      <c r="D224" s="44">
+      <c r="D224" s="7">
         <v>106783</v>
       </c>
-      <c r="E224" s="44">
+      <c r="E224" s="7">
         <v>1311</v>
       </c>
-      <c r="F224" s="44" t="s">
+      <c r="F224" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G224" s="44" t="s">
+      <c r="G224" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H224" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I224" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J224" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K224" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L224" s="44" t="s">
+      <c r="H224" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I224" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J224" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K224" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L224" s="7" t="s">
         <v>1340</v>
       </c>
-      <c r="M224" s="45"/>
-      <c r="N224" s="44"/>
-      <c r="O224" s="44"/>
-      <c r="P224" s="44"/>
-    </row>
-    <row r="225" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B225" s="44" t="s">
+      <c r="M224" s="2"/>
+      <c r="N224" s="7"/>
+      <c r="O224" s="7"/>
+      <c r="P224" s="7"/>
+    </row>
+    <row r="225" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A225" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B225" s="7" t="s">
         <v>1308</v>
       </c>
-      <c r="C225" s="44">
+      <c r="C225" s="7">
         <v>106777</v>
       </c>
-      <c r="D225" s="44">
+      <c r="D225" s="7">
         <v>107133</v>
       </c>
-      <c r="E225" s="44">
+      <c r="E225" s="7">
         <v>357</v>
       </c>
-      <c r="F225" s="44"/>
-      <c r="G225" s="44"/>
-      <c r="H225" s="44"/>
-      <c r="I225" s="44"/>
-      <c r="J225" s="44"/>
-      <c r="K225" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L225" s="44"/>
-      <c r="M225" s="45"/>
-      <c r="N225" s="44"/>
-      <c r="O225" s="44"/>
-      <c r="P225" s="44"/>
-    </row>
-    <row r="226" spans="1:16" s="46" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A226" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B226" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C226" s="44">
+      <c r="F225" s="7"/>
+      <c r="G225" s="7"/>
+      <c r="H225" s="7"/>
+      <c r="I225" s="7"/>
+      <c r="J225" s="7"/>
+      <c r="K225" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L225" s="7"/>
+      <c r="M225" s="2"/>
+      <c r="N225" s="7"/>
+      <c r="O225" s="7"/>
+      <c r="P225" s="7"/>
+    </row>
+    <row r="226" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A226" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B226" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C226" s="7">
         <v>106846</v>
       </c>
-      <c r="D226" s="44">
+      <c r="D226" s="7">
         <v>107133</v>
       </c>
-      <c r="E226" s="44">
+      <c r="E226" s="7">
         <v>288</v>
       </c>
-      <c r="F226" s="44" t="s">
+      <c r="F226" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G226" s="44" t="str">
+      <c r="G226" s="7" t="str">
         <f>B225</f>
         <v>RING-finger domain-containing E3 protein CDS</v>
       </c>
-      <c r="H226" s="47">
+      <c r="H226" s="11">
         <v>106777</v>
       </c>
-      <c r="I226" s="44">
+      <c r="I226" s="7">
         <v>107133</v>
       </c>
-      <c r="J226" s="47">
+      <c r="J226" s="11">
         <v>357</v>
       </c>
-      <c r="K226" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L226" s="44" t="s">
+      <c r="K226" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L226" s="7" t="s">
         <v>1341</v>
       </c>
-      <c r="M226" s="45" t="s">
-        <v>1390</v>
-      </c>
-      <c r="N226" s="44"/>
-      <c r="O226" s="44"/>
-      <c r="P226" s="44"/>
+      <c r="M226" s="2" t="s">
+        <v>1388</v>
+      </c>
+      <c r="N226" s="7"/>
+      <c r="O226" s="7"/>
+      <c r="P226" s="7"/>
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227" s="7" t="s">
@@ -56802,79 +56792,79 @@
       <c r="O232" s="7"/>
       <c r="P232" s="7"/>
     </row>
-    <row r="233" spans="1:16" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B233" s="44" t="s">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A233" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B233" s="7" t="s">
         <v>1346</v>
       </c>
-      <c r="C233" s="44">
+      <c r="C233" s="7">
         <v>109124</v>
       </c>
-      <c r="D233" s="44">
+      <c r="D233" s="7">
         <v>109318</v>
       </c>
-      <c r="E233" s="44">
+      <c r="E233" s="7">
         <v>195</v>
       </c>
-      <c r="F233" s="44"/>
-      <c r="G233" s="44"/>
-      <c r="H233" s="44"/>
-      <c r="I233" s="44"/>
-      <c r="J233" s="44"/>
-      <c r="K233" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="L233" s="44"/>
-      <c r="M233" s="45"/>
-      <c r="N233" s="44"/>
-      <c r="O233" s="44"/>
-      <c r="P233" s="44"/>
-    </row>
-    <row r="234" spans="1:16" s="46" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A234" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B234" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C234" s="44">
+      <c r="F233" s="7"/>
+      <c r="G233" s="7"/>
+      <c r="H233" s="7"/>
+      <c r="I233" s="7"/>
+      <c r="J233" s="7"/>
+      <c r="K233" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L233" s="7"/>
+      <c r="M233" s="2"/>
+      <c r="N233" s="7"/>
+      <c r="O233" s="7"/>
+      <c r="P233" s="7"/>
+    </row>
+    <row r="234" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A234" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B234" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C234" s="7">
         <v>109018</v>
       </c>
-      <c r="D234" s="44">
+      <c r="D234" s="7">
         <v>109398</v>
       </c>
-      <c r="E234" s="44">
+      <c r="E234" s="7">
         <v>381</v>
       </c>
-      <c r="F234" s="44" t="s">
+      <c r="F234" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G234" s="44" t="s">
+      <c r="G234" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H234" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I234" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J234" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="K234" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L234" s="44" t="s">
+      <c r="H234" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I234" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J234" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K234" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L234" s="7" t="s">
         <v>1347</v>
       </c>
-      <c r="M234" s="45" t="s">
-        <v>1391</v>
-      </c>
-      <c r="N234" s="44"/>
-      <c r="O234" s="44"/>
-      <c r="P234" s="44"/>
+      <c r="M234" s="2" t="s">
+        <v>1389</v>
+      </c>
+      <c r="N234" s="7"/>
+      <c r="O234" s="7"/>
+      <c r="P234" s="7"/>
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A235" s="7" t="s">

</xml_diff>